<commit_message>
feat: add image scaling for screenshots and externalize key paths for user config
- Installed image-size for screenshot scaling
- Updated excel-template.xlsx with new formatting
- Refactored excel-writer-util to support image scaling
- Created text-writer-util to separate text writing logic
- Relocated text report name, Excel template path, and Excel output name to lighthouse.config.ts
- Updated report-path-util to use externalized text report name
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cheqteams-my.sharepoint.com/personal/vwlabajo_cheqsystems_com/Documents/Documents/Team - Performance Testing/PT - Documentation/CheQ Website Production Page Speed Insight/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85A7CDF9-1448-41CA-8A15-D50BB63BA09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{8EA300FF-E831-4373-BB35-1174E74F1E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{573A2E2B-B5CE-41B0-B334-BA4A05AE6729}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C37E2E45-7E9A-43D5-A28B-C770F3703849}"/>
   </bookViews>
@@ -28,35 +28,24 @@
     <definedName name="performanceRange" localSheetId="0">Summary!$L$6:$L$35</definedName>
     <definedName name="performanceValueRange" comment="This variable refers to the performance of all pages, for devices, cache, and without cache.">Summary!$L$6,Summary!$L$7,Summary!$L$10,Summary!$L$11,Summary!$L$14,Summary!$L$15,Summary!$L$18,Summary!$L$19,Summary!$L$22,Summary!$L$23,Summary!$L$26,Summary!$L$27,Summary!$L$30,Summary!$L$31</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -73,10 +62,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="47">
   <si>
-    <t>PageSpeed Insights</t>
+    <t>Lighthouse Insights</t>
   </si>
   <si>
-    <t>Production</t>
+    <t>URLs</t>
   </si>
   <si>
     <t xml:space="preserve">Performance </t>
@@ -88,10 +77,10 @@
     <t>Device</t>
   </si>
   <si>
-    <t>With Cache</t>
+    <t>Normal</t>
   </si>
   <si>
-    <t>Without Cache</t>
+    <t>Incognito</t>
   </si>
   <si>
     <t>Best</t>
@@ -106,10 +95,10 @@
     <t>Device Selector</t>
   </si>
   <si>
-    <t>Cell with Highest</t>
+    <t>Cell normal Highest</t>
   </si>
   <si>
-    <t>Cell with Lowest</t>
+    <t>Cell normal Lowest</t>
   </si>
   <si>
     <t>Device:</t>
@@ -175,7 +164,7 @@
     <t>Record performance value location:</t>
   </si>
   <si>
-    <t>With and Without Cache Value Location:</t>
+    <t>normal and incognito Value Location:</t>
   </si>
   <si>
     <t>Cache Value:</t>
@@ -222,7 +211,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,12 +283,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -313,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE02B2B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,9 +704,6 @@
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -727,31 +713,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -773,10 +759,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,74 +781,80 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="5" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -887,13 +879,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -902,9 +894,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -926,8 +915,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -946,8 +935,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -966,8 +955,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -986,8 +975,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1006,8 +995,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1026,8 +1015,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1046,8 +1035,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1066,8 +1055,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1075,6 +1064,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE02B2B"/>
+      <color rgb="FFFF2424"/>
+      <color rgb="FFFF4545"/>
+      <color rgb="FFDE5757"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFFF5050"/>
     </mruColors>
@@ -1828,35 +1821,35 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="101.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="33.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="31" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" style="31" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" style="31" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="31" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="31" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" style="31" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="101.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="33.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="24.88671875" style="30" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" style="30" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" style="30" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" style="30" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" style="30" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" style="30" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1"/>
-    <row r="2" spans="1:15" ht="15" thickBot="1">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D2" s="55" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="56"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1">
-      <c r="A3" s="4"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
       <c r="B3" s="57" t="s">
         <v>1</v>
       </c>
@@ -1865,36 +1858,36 @@
         <v>2</v>
       </c>
       <c r="E3" s="60"/>
-      <c r="F3" s="6"/>
-      <c r="J3" s="42"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1">
-      <c r="B4" s="8" t="s">
+      <c r="F3" s="5"/>
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="J5" s="35" t="s">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="J5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M5" t="s">
@@ -1907,896 +1900,896 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="6"/>
+    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J6&amp;" devices "&amp; J7 &amp;",  at  "&amp; L6
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K6 &amp;" devices "&amp; K7 &amp;", at "&amp;L7
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B7&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 01_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="36" t="str" cm="1">
+      <c r="J6" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT(M6)</f>
         <v>Desktop</v>
       </c>
-      <c r="K6" s="38" t="str" cm="1">
+      <c r="K6" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDIRECT(M7)</f>
         <v>Desktop</v>
       </c>
-      <c r="L6" s="40">
+      <c r="L6" s="39">
         <f>MAX(D7:E8)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="31" t="str">
+      <c r="M6" s="30" t="str">
         <f>IF(LEFT(N6,1)="D",
     CHAR(CODE(LEFT(N6,1)) - 1) &amp; MID(N6,2,99),
     CHAR(CODE(LEFT(N6,1)) - 2) &amp; MID(N6,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="N6" s="34" t="str" cm="1">
+      <c r="N6" s="33" t="str" cm="1">
         <f t="array" ref="N6">ADDRESS(MIN(IF(D7:E8=L6,ROW(D7:E8))), MIN(IF(D7:E8=L6,COLUMN(D7:E8))), 4)</f>
         <v>D7</v>
       </c>
-      <c r="O6" s="34" t="str" cm="1">
+      <c r="O6" s="33" t="str" cm="1">
         <f t="array" ref="O6">ADDRESS(MIN(IF(D7:E8=L7,ROW(D7:E8))), MIN(IF(D7:E8=L7,COLUMN(D7:E8))), 4)</f>
         <v>D7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="6"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="51"/>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="36" t="str">
-        <f ca="1">IF(J6="Desktop",IF(D7=E7,"with and without cache",(IF(D7&gt;E7,"with cache","without cache"))),IF(D8=E8,"with and without cache",(IF(D8&gt;E8,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K7" s="38" t="str">
-        <f ca="1">IF(K6="Desktop",IF(D7=E7,"with and without cache",IF(D7&lt;E7,"with cache","without cache")),IF(D8=E8,"with and without cache",IF(D8&lt;E8,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L7" s="39">
+      <c r="J7" s="35" t="str">
+        <f ca="1">IF(J6="Desktop",IF(D7=E7,"normal and incognito",(IF(D7&gt;E7,"normal","incognito"))),IF(D8=E8,"normal and incognito",(IF(D8&gt;E8,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K7" s="37" t="str">
+        <f ca="1">IF(K6="Desktop",IF(D7=E7,"normal and incognito",IF(D7&lt;E7,"normal","incognito")),IF(D8=E8,"normal and incognito",IF(D8&lt;E8,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L7" s="38">
         <f>MIN(D7:E8)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="34" t="str">
+      <c r="M7" s="33" t="str">
         <f>IF(LEFT(O6,1)="D",
     CHAR(CODE(LEFT(O6,1)) - 1) &amp; MID(O6,2,99),
     CHAR(CODE(LEFT(O6,1)) - 2) &amp; MID(O6,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-    </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1">
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+    </row>
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="54"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="6"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="52"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="L9" s="30" t="s">
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="L9" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="6"/>
+    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J10&amp;" devices "&amp; J11 &amp;",  at  "&amp; L10
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K10 &amp;" devices "&amp; K11 &amp;", at "&amp;L11
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B11&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 02_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="36" t="str" cm="1">
+      <c r="J10" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT(M10)</f>
         <v>Desktop</v>
       </c>
-      <c r="K10" s="38" t="str" cm="1">
+      <c r="K10" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">INDIRECT(M11)</f>
         <v>Desktop</v>
       </c>
-      <c r="L10" s="40">
+      <c r="L10" s="39">
         <f>MAX(D11:E12)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="31" t="str">
+      <c r="M10" s="30" t="str">
         <f>IF(LEFT(N10,1)="D",
     CHAR(CODE(LEFT(N10,1)) - 1) &amp; MID(N10,2,99),
     CHAR(CODE(LEFT(N10,1)) - 2) &amp; MID(N10,2,99)
 )</f>
         <v>C11</v>
       </c>
-      <c r="N10" s="34" t="str" cm="1">
+      <c r="N10" s="33" t="str" cm="1">
         <f t="array" ref="N10">ADDRESS(MIN(IF(D11:E12=L10,ROW(D11:E12))), MIN(IF(D11:E12=L10,COLUMN(D11:E12))), 4)</f>
         <v>D11</v>
       </c>
-      <c r="O10" s="34" t="str" cm="1">
+      <c r="O10" s="33" t="str" cm="1">
         <f t="array" ref="O10">ADDRESS(MIN(IF(D11:E12=L11,ROW(D11:E12))), MIN(IF(D11:E12=L11,COLUMN(D11:E12))), 4)</f>
         <v>D11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1">
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
       <c r="G11" s="51"/>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="36" t="str">
-        <f ca="1">IF(J10="Desktop",IF(D11=E11,"with and without cache",(IF(D11&gt;E11,"with cache","without cache"))),IF(D12=E12,"with and without cache",(IF(D12&gt;E12,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K11" s="38" t="str">
-        <f ca="1">IF(K10="Desktop",IF(D11=E11,"with and without cache",IF(D11&lt;E11,"with cache","without cache")),IF(D12=E12,"with and without cache",IF(D12&lt;E12,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L11" s="39">
+      <c r="J11" s="35" t="str">
+        <f ca="1">IF(J10="Desktop",IF(D11=E11,"normal and incognito",(IF(D11&gt;E11,"normal","incognito"))),IF(D12=E12,"normal and incognito",(IF(D12&gt;E12,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K11" s="37" t="str">
+        <f ca="1">IF(K10="Desktop",IF(D11=E11,"normal and incognito",IF(D11&lt;E11,"normal","incognito")),IF(D12=E12,"normal and incognito",IF(D12&lt;E12,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L11" s="38">
         <f>MIN(D11:E12)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="34" t="str">
+      <c r="M11" s="33" t="str">
         <f>IF(LEFT(O10,1)="D",
     CHAR(CODE(LEFT(O10,1)) - 1) &amp; MID(O10,2,99),
     CHAR(CODE(LEFT(O10,1)) - 2) &amp; MID(O10,2,99)
 )</f>
         <v>C11</v>
       </c>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-    </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1">
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="54"/>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="52"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="L13" s="30" t="s">
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+    </row>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="L13" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="6"/>
+    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J14&amp;" devices "&amp; J15 &amp;",  at  "&amp; L14
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K14 &amp;" devices "&amp; K15 &amp;", at "&amp;L15
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B15&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 03_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="36" t="str" cm="1">
+      <c r="J14" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT(M14)</f>
         <v>Desktop</v>
       </c>
-      <c r="K14" s="38" t="str" cm="1">
+      <c r="K14" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K14" ca="1">INDIRECT(M15)</f>
         <v>Desktop</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="39">
         <f>MAX(D15:E16)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="31" t="str">
+      <c r="M14" s="30" t="str">
         <f>IF(LEFT(N14,1)="D",
     CHAR(CODE(LEFT(N14,1)) - 1) &amp; MID(N14,2,99),
     CHAR(CODE(LEFT(N14,1)) - 2) &amp; MID(N14,2,99)
 )</f>
         <v>C15</v>
       </c>
-      <c r="N14" s="34" t="str" cm="1">
+      <c r="N14" s="33" t="str" cm="1">
         <f t="array" ref="N14">ADDRESS(MIN(IF(D15:E16=L14,ROW(D15:E16))), MIN(IF(D15:E16=L14,COLUMN(D15:E16))), 4)</f>
         <v>D15</v>
       </c>
-      <c r="O14" s="34" t="str" cm="1">
+      <c r="O14" s="33" t="str" cm="1">
         <f t="array" ref="O14">ADDRESS(MIN(IF(D15:E16=L15,ROW(D15:E16))), MIN(IF(D15:E16=L15,COLUMN(D15:E16))), 4)</f>
         <v>D15</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="6"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="51"/>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="36" t="str">
-        <f ca="1">IF(J14="Desktop",IF(D15=E15,"with and without cache",(IF(D15&gt;E15,"with cache","without cache"))),IF(D16=E16,"with and without cache",(IF(D16&gt;E16,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K15" s="38" t="str">
-        <f ca="1">IF(K14="Desktop",IF(D15=E15,"with and without cache",IF(D15&lt;E15,"with cache","without cache")),IF(D16=E16,"with and without cache",IF(D16&lt;E16,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L15" s="39">
+      <c r="J15" s="35" t="str">
+        <f ca="1">IF(J14="Desktop",IF(D15=E15,"normal and incognito",(IF(D15&gt;E15,"normal","incognito"))),IF(D16=E16,"normal and incognito",(IF(D16&gt;E16,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K15" s="37" t="str">
+        <f ca="1">IF(K14="Desktop",IF(D15=E15,"normal and incognito",IF(D15&lt;E15,"normal","incognito")),IF(D16=E16,"normal and incognito",IF(D16&lt;E16,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L15" s="38">
         <f>MIN(D15:E16)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="34" t="str">
+      <c r="M15" s="33" t="str">
         <f>IF(LEFT(O14,1)="D",
     CHAR(CODE(LEFT(O14,1)) - 1) &amp; MID(O14,2,99),
     CHAR(CODE(LEFT(O14,1)) - 2) &amp; MID(O14,2,99)
 )</f>
         <v>C15</v>
       </c>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1">
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="54"/>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="52"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-    </row>
-    <row r="17" spans="2:15" ht="15" thickBot="1">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="L17" s="30" t="s">
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+    </row>
+    <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="L17" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="6"/>
+    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J18&amp;" devices "&amp; J19 &amp;",  at  "&amp; L18
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K18 &amp;" devices "&amp; K19 &amp;", at "&amp;L19
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B19&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 04_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="36" t="str" cm="1">
+      <c r="J18" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">INDIRECT(M18)</f>
         <v>Desktop</v>
       </c>
-      <c r="K18" s="38" t="str" cm="1">
+      <c r="K18" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K18" ca="1">INDIRECT(M19)</f>
         <v>Desktop</v>
       </c>
-      <c r="L18" s="40">
+      <c r="L18" s="39">
         <f>MAX(D19:E20)</f>
         <v>0</v>
       </c>
-      <c r="M18" s="31" t="str">
+      <c r="M18" s="30" t="str">
         <f>IF(LEFT(N18,1)="D",
     CHAR(CODE(LEFT(N18,1)) - 1) &amp; MID(N18,2,99),
     CHAR(CODE(LEFT(N18,1)) - 2) &amp; MID(N18,2,99)
 )</f>
         <v>C19</v>
       </c>
-      <c r="N18" s="34" t="str" cm="1">
+      <c r="N18" s="33" t="str" cm="1">
         <f t="array" ref="N18">ADDRESS(MIN(IF(D19:E20=L18,ROW(D19:E20))), MIN(IF(D19:E20=L18,COLUMN(D19:E20))), 4)</f>
         <v>D19</v>
       </c>
-      <c r="O18" s="34" t="str" cm="1">
+      <c r="O18" s="33" t="str" cm="1">
         <f t="array" ref="O18">ADDRESS(MIN(IF(D19:E20=L19,ROW(D19:E20))), MIN(IF(D19:E20=L19,COLUMN(D19:E20))), 4)</f>
         <v>D19</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15" thickBot="1">
+    <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="6"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="51"/>
-      <c r="I19" s="30" t="s">
+      <c r="I19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="36" t="str">
-        <f ca="1">IF(J18="Desktop",IF(D19=E19,"with and without cache",(IF(D19&gt;E19,"with cache","without cache"))),IF(D20=E20,"with and without cache",(IF(D20&gt;E20,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K19" s="38" t="str">
-        <f ca="1">IF(K18="Desktop",IF(D19=E19,"with and without cache",IF(D19&lt;E19,"with cache","without cache")),IF(D20=E20,"with and without cache",IF(D20&lt;E20,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L19" s="39">
+      <c r="J19" s="35" t="str">
+        <f ca="1">IF(J18="Desktop",IF(D19=E19,"normal and incognito",(IF(D19&gt;E19,"normal","incognito"))),IF(D20=E20,"normal and incognito",(IF(D20&gt;E20,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K19" s="37" t="str">
+        <f ca="1">IF(K18="Desktop",IF(D19=E19,"normal and incognito",IF(D19&lt;E19,"normal","incognito")),IF(D20=E20,"normal and incognito",IF(D20&lt;E20,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L19" s="38">
         <f>MIN(D19:E20)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="34" t="str">
+      <c r="M19" s="33" t="str">
         <f>IF(LEFT(O18,1)="D",
     CHAR(CODE(LEFT(O18,1)) - 1) &amp; MID(O18,2,99),
     CHAR(CODE(LEFT(O18,1)) - 2) &amp; MID(O18,2,99)
 )</f>
         <v>C19</v>
       </c>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-    </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1">
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+    </row>
+    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="54"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="6"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="52"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-    </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="L21" s="30" t="s">
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+    </row>
+    <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="L21" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
     </row>
-    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="6"/>
+    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J22&amp;" devices "&amp; J23 &amp;",  at  "&amp; L22
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K22 &amp;" devices "&amp; K23 &amp;", at "&amp;L23
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B23&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 05_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I22" s="30" t="s">
+      <c r="I22" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="36" t="str" cm="1">
+      <c r="J22" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">INDIRECT(M22)</f>
         <v>Desktop</v>
       </c>
-      <c r="K22" s="38" t="str" cm="1">
+      <c r="K22" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K22" ca="1">INDIRECT(M23)</f>
         <v>Desktop</v>
       </c>
-      <c r="L22" s="40">
+      <c r="L22" s="39">
         <f>MAX(D23:E24)</f>
         <v>0</v>
       </c>
-      <c r="M22" s="31" t="str">
+      <c r="M22" s="30" t="str">
         <f>IF(LEFT(N22,1)="D",
     CHAR(CODE(LEFT(N22,1)) - 1) &amp; MID(N22,2,99),
     CHAR(CODE(LEFT(N22,1)) - 2) &amp; MID(N22,2,99)
 )</f>
         <v>C23</v>
       </c>
-      <c r="N22" s="34" t="str" cm="1">
+      <c r="N22" s="33" t="str" cm="1">
         <f t="array" ref="N22">ADDRESS(MIN(IF(D23:E24=L22,ROW(D23:E24))), MIN(IF(D23:E24=L22,COLUMN(D23:E24))), 4)</f>
         <v>D23</v>
       </c>
-      <c r="O22" s="34" t="str" cm="1">
+      <c r="O22" s="33" t="str" cm="1">
         <f t="array" ref="O22">ADDRESS(MIN(IF(D23:E24=L23,ROW(D23:E24))), MIN(IF(D23:E24=L23,COLUMN(D23:E24))), 4)</f>
         <v>D23</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="15" thickBot="1">
+    <row r="23" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="6"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="51"/>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="36" t="str">
-        <f ca="1">IF(J22="Desktop",IF(D23=E23,"with and without cache",(IF(D23&gt;E23,"with cache","without cache"))),IF(D24=E24,"with and without cache",(IF(D24&gt;E24,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K23" s="38" t="str">
-        <f ca="1">IF(K22="Desktop",IF(D23=E23,"with and without cache",IF(D23&lt;E23,"with cache","without cache")),IF(D24=E24,"with and without cache",IF(D24&lt;E24,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L23" s="39">
+      <c r="J23" s="35" t="str">
+        <f ca="1">IF(J22="Desktop",IF(D23=E23,"normal and incognito",(IF(D23&gt;E23,"normal","incognito"))),IF(D24=E24,"normal and incognito",(IF(D24&gt;E24,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K23" s="37" t="str">
+        <f ca="1">IF(K22="Desktop",IF(D23=E23,"normal and incognito",IF(D23&lt;E23,"normal","incognito")),IF(D24=E24,"normal and incognito",IF(D24&lt;E24,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L23" s="38">
         <f>MIN(D23:E24)</f>
         <v>0</v>
       </c>
-      <c r="M23" s="34" t="str">
+      <c r="M23" s="33" t="str">
         <f>IF(LEFT(O22,1)="D",
     CHAR(CODE(LEFT(O22,1)) - 1) &amp; MID(O22,2,99),
     CHAR(CODE(LEFT(O22,1)) - 2) &amp; MID(O22,2,99)
 )</f>
         <v>C23</v>
       </c>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-    </row>
-    <row r="24" spans="2:15" ht="15" thickBot="1">
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+    </row>
+    <row r="24" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="54"/>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="6"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="52"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-    </row>
-    <row r="25" spans="2:15" ht="15" thickBot="1">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="L25" s="30" t="s">
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+    </row>
+    <row r="25" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="L25" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
     </row>
-    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="6"/>
+    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J26&amp;" devices "&amp; J27 &amp;",  at  "&amp; L26
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K26 &amp;" devices "&amp; K27 &amp;", at "&amp;L27
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B27&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 06_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="36" t="str" cm="1">
+      <c r="J26" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J26" ca="1">INDIRECT(M26)</f>
         <v>Desktop</v>
       </c>
-      <c r="K26" s="38" t="str" cm="1">
+      <c r="K26" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K26" ca="1">INDIRECT(M27)</f>
         <v>Desktop</v>
       </c>
-      <c r="L26" s="40">
+      <c r="L26" s="39">
         <f>MAX(D27:E28)</f>
         <v>0</v>
       </c>
-      <c r="M26" s="31" t="str">
+      <c r="M26" s="30" t="str">
         <f>IF(LEFT(N26,1)="D",
     CHAR(CODE(LEFT(N26,1)) - 1) &amp; MID(N26,2,99),
     CHAR(CODE(LEFT(N26,1)) - 2) &amp; MID(N26,2,99)
 )</f>
         <v>C27</v>
       </c>
-      <c r="N26" s="34" t="str" cm="1">
+      <c r="N26" s="33" t="str" cm="1">
         <f t="array" ref="N26">ADDRESS(MIN(IF(D27:E28=L26,ROW(D27:E28))), MIN(IF(D27:E28=L26,COLUMN(D27:E28))), 4)</f>
         <v>D27</v>
       </c>
-      <c r="O26" s="34" t="str" cm="1">
+      <c r="O26" s="33" t="str" cm="1">
         <f t="array" ref="O26">ADDRESS(MIN(IF(D27:E28=L27,ROW(D27:E28))), MIN(IF(D27:E28=L27,COLUMN(D27:E28))), 4)</f>
         <v>D27</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="15" thickBot="1">
+    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="6"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="51"/>
-      <c r="I27" s="30" t="s">
+      <c r="I27" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J27" s="36" t="str">
-        <f ca="1">IF(J26="Desktop",IF(D27=E27,"with and without cache",(IF(D27&gt;E27,"with cache","without cache"))),IF(D28=E28,"with and without cache",(IF(D28&gt;E28,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K27" s="38" t="str">
-        <f ca="1">IF(K26="Desktop",IF(D27=E27,"with and without cache",IF(D27&lt;E27,"with cache","without cache")),IF(D28=E28,"with and without cache",IF(D28&lt;E28,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L27" s="39">
+      <c r="J27" s="35" t="str">
+        <f ca="1">IF(J26="Desktop",IF(D27=E27,"normal and incognito",(IF(D27&gt;E27,"normal","incognito"))),IF(D28=E28,"normal and incognito",(IF(D28&gt;E28,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K27" s="37" t="str">
+        <f ca="1">IF(K26="Desktop",IF(D27=E27,"normal and incognito",IF(D27&lt;E27,"normal","incognito")),IF(D28=E28,"normal and incognito",IF(D28&lt;E28,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L27" s="38">
         <f>MIN(D27:E28)</f>
         <v>0</v>
       </c>
-      <c r="M27" s="34" t="str">
+      <c r="M27" s="33" t="str">
         <f>IF(LEFT(O26,1)="D",
     CHAR(CODE(LEFT(O26,1)) - 1) &amp; MID(O26,2,99),
     CHAR(CODE(LEFT(O26,1)) - 2) &amp; MID(O26,2,99)
 )</f>
         <v>C27</v>
       </c>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-    </row>
-    <row r="28" spans="2:15" ht="15" thickBot="1">
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="54"/>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="6"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="52"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-    </row>
-    <row r="29" spans="2:15" ht="15" thickBot="1">
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="L29" s="30" t="s">
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+    </row>
+    <row r="29" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="L29" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
     </row>
-    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="6"/>
+    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J30&amp;" devices "&amp; J31 &amp;",  at  "&amp; L30
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K30 &amp;" devices "&amp; K31 &amp;", at "&amp;L31
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B31&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 07_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I30" s="30" t="s">
+      <c r="I30" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J30" s="36" t="str" cm="1">
+      <c r="J30" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J30" ca="1">INDIRECT(M30)</f>
         <v>Desktop</v>
       </c>
-      <c r="K30" s="38" t="str" cm="1">
+      <c r="K30" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K30" ca="1">INDIRECT(M31)</f>
         <v>Desktop</v>
       </c>
-      <c r="L30" s="40">
+      <c r="L30" s="39">
         <f>MAX(D31:E32)</f>
         <v>0</v>
       </c>
-      <c r="M30" s="31" t="str">
+      <c r="M30" s="30" t="str">
         <f>IF(LEFT(N30,1)="D",
     CHAR(CODE(LEFT(N30,1)) - 1) &amp; MID(N30,2,99),
     CHAR(CODE(LEFT(N30,1)) - 2) &amp; MID(N30,2,99)
 )</f>
         <v>C31</v>
       </c>
-      <c r="N30" s="34" t="str" cm="1">
+      <c r="N30" s="33" t="str" cm="1">
         <f t="array" ref="N30">ADDRESS(MIN(IF(D31:E32=L30,ROW(D31:E32))), MIN(IF(D31:E32=L30,COLUMN(D31:E32))), 4)</f>
         <v>D31</v>
       </c>
-      <c r="O30" s="34" t="str" cm="1">
+      <c r="O30" s="33" t="str" cm="1">
         <f t="array" ref="O30">ADDRESS(MIN(IF(D31:E32=L31,ROW(D31:E32))), MIN(IF(D31:E32=L31,COLUMN(D31:E32))), 4)</f>
         <v>D31</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="15" thickBot="1">
+    <row r="31" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="6"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="51"/>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="36" t="str">
-        <f ca="1">IF(J30="Desktop",IF(D31=E31,"with and without cache",(IF(D31&gt;E31,"with cache","without cache"))),IF(D32=E32,"with and without cache",(IF(D32&gt;E32,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K31" s="38" t="str">
-        <f ca="1">IF(K30="Desktop",IF(D31=E31,"with and without cache",IF(D31&lt;E31,"with cache","without cache")),IF(D32=E32,"with and without cache",IF(D32&lt;E32,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L31" s="39">
+      <c r="J31" s="35" t="str">
+        <f ca="1">IF(J30="Desktop",IF(D31=E31,"normal and incognito",(IF(D31&gt;E31,"normal","incognito"))),IF(D32=E32,"normal and incognito",(IF(D32&gt;E32,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K31" s="37" t="str">
+        <f ca="1">IF(K30="Desktop",IF(D31=E31,"normal and incognito",IF(D31&lt;E31,"normal","incognito")),IF(D32=E32,"normal and incognito",IF(D32&lt;E32,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L31" s="38">
         <f>MIN(D31:E32)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="34" t="str">
+      <c r="M31" s="33" t="str">
         <f>IF(LEFT(O30,1)="D",
     CHAR(CODE(LEFT(O30,1)) - 1) &amp; MID(O30,2,99),
     CHAR(CODE(LEFT(O30,1)) - 2) &amp; MID(O30,2,99)
 )</f>
         <v>C31</v>
       </c>
-      <c r="N31" s="34"/>
-      <c r="O31" s="34"/>
-    </row>
-    <row r="32" spans="2:15">
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="54"/>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="6"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="52"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-    </row>
-    <row r="33" spans="2:15">
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="43"/>
-      <c r="L33" s="30" t="s">
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="42"/>
+      <c r="L33" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M33"/>
       <c r="N33"/>
       <c r="O33"/>
     </row>
-    <row r="34" spans="2:15" ht="14.45" customHeight="1">
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="6"/>
+    <row r="34" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J34&amp;" devices "&amp; J35 &amp;",  at  "&amp; L34
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K34 &amp;" devices "&amp; K35 &amp;", at "&amp;L35
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B35&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 08_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I34" s="30" t="s">
+      <c r="I34" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J34" s="36" t="str" cm="1">
+      <c r="J34" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J34" ca="1">INDIRECT(M34)</f>
         <v>Desktop</v>
       </c>
-      <c r="K34" s="38" t="str" cm="1">
+      <c r="K34" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K34" ca="1">INDIRECT(M35)</f>
         <v>Desktop</v>
       </c>
-      <c r="L34" s="40">
+      <c r="L34" s="39">
         <f>MAX(D35:E36)</f>
         <v>0</v>
       </c>
-      <c r="M34" s="31" t="str">
+      <c r="M34" s="30" t="str">
         <f>IF(LEFT(N34,1)="D",
     CHAR(CODE(LEFT(N34,1)) - 1) &amp; MID(N34,2,99),
     CHAR(CODE(LEFT(N34,1)) - 2) &amp; MID(N34,2,99)
 )</f>
         <v>C35</v>
       </c>
-      <c r="N34" s="34" t="str" cm="1">
+      <c r="N34" s="33" t="str" cm="1">
         <f t="array" ref="N34">ADDRESS(MIN(IF(D35:E36=L34,ROW(D35:E36))), MIN(IF(D35:E36=L34,COLUMN(D35:E36))), 4)</f>
         <v>D35</v>
       </c>
-      <c r="O34" s="34" t="str" cm="1">
+      <c r="O34" s="33" t="str" cm="1">
         <f t="array" ref="O34">ADDRESS(MIN(IF(D35:E36=L35,ROW(D35:E36))), MIN(IF(D35:E36=L35,COLUMN(D35:E36))), 4)</f>
         <v>D35</v>
       </c>
     </row>
-    <row r="35" spans="2:15">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="6"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="51"/>
-      <c r="I35" s="30" t="s">
+      <c r="I35" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J35" s="36" t="str">
-        <f ca="1">IF(J34="Desktop",IF(D35=E35,"with and without cache",(IF(D35&gt;E35,"with cache","without cache"))),IF(D36=E36,"with and without cache",(IF(D36&gt;E36,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K35" s="38" t="str">
-        <f ca="1">IF(K34="Desktop",IF(D35=E35,"with and without cache",IF(D35&lt;E35,"with cache","without cache")),IF(D36=E36,"with and without cache",IF(D36&lt;E36,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L35" s="39">
+      <c r="J35" s="35" t="str">
+        <f ca="1">IF(J34="Desktop",IF(D35=E35,"normal and incognito",(IF(D35&gt;E35,"normal","incognito"))),IF(D36=E36,"normal and incognito",(IF(D36&gt;E36,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K35" s="37" t="str">
+        <f ca="1">IF(K34="Desktop",IF(D35=E35,"normal and incognito",IF(D35&lt;E35,"normal","incognito")),IF(D36=E36,"normal and incognito",IF(D36&lt;E36,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L35" s="38">
         <f>MIN(D35:E36)</f>
         <v>0</v>
       </c>
-      <c r="M35" s="34" t="str">
+      <c r="M35" s="33" t="str">
         <f>IF(LEFT(O34,1)="D",
     CHAR(CODE(LEFT(O34,1)) - 1) &amp; MID(O34,2,99),
     CHAR(CODE(LEFT(O34,1)) - 2) &amp; MID(O34,2,99)
 )</f>
         <v>C35</v>
       </c>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34"/>
-    </row>
-    <row r="36" spans="2:15">
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36" s="54"/>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="6"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="52"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-    </row>
-    <row r="37" spans="2:15">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="34"/>
-    </row>
-    <row r="38" spans="2:15" ht="14.45" customHeight="1">
-      <c r="C38" s="12" t="s">
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+    </row>
+    <row r="38" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="6"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="50" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">IFERROR(
     "The best recorded performance score was in the " &amp; J46 &amp; " page for " &amp; INDIRECT(J43) &amp; " devices " &amp; J42 &amp; ", at " &amp; J39 &amp; CHAR(10) &amp;
@@ -2807,140 +2800,140 @@
 )</f>
         <v>Kindly, fill the Performance Score first!</v>
       </c>
-      <c r="I38" s="30" t="s">
+      <c r="I38" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J38" s="32" t="s">
+      <c r="J38" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K38" s="32" t="s">
+      <c r="K38" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="34"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34"/>
-    </row>
-    <row r="39" spans="2:15">
-      <c r="C39" s="13" t="s">
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+      <c r="O38" s="33"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C39" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="6"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="51"/>
-      <c r="I39" s="30" t="s">
+      <c r="I39" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J39" s="32">
+      <c r="J39" s="31">
         <f>MAX(performanceRange)</f>
         <v>0</v>
       </c>
-      <c r="K39" s="33">
+      <c r="K39" s="32">
         <f>MIN(performanceRange)</f>
         <v>0</v>
       </c>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-    </row>
-    <row r="40" spans="2:15">
-      <c r="C40" s="14" t="s">
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C40" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="6"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="51"/>
-      <c r="I40" s="30" t="s">
+      <c r="I40" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="32" t="str" cm="1">
+      <c r="J40" s="31" t="str" cm="1">
         <f t="array" ref="J40">ADDRESS(MIN(IF(D7:E36=J39,ROW(D7:E36))), MIN(IF(D7:E36=J39,COLUMN(D7:E36))), 4)</f>
         <v>D7</v>
       </c>
-      <c r="K40" s="32" t="str" cm="1">
+      <c r="K40" s="31" t="str" cm="1">
         <f t="array" ref="K40">ADDRESS(MIN(IF(D7:E36=K39,ROW(D7:E36))), MIN(IF(D7:E36=K39,COLUMN(D7:E36))), 4)</f>
         <v>D7</v>
       </c>
-      <c r="L40" s="34"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
-      <c r="O40" s="34"/>
-    </row>
-    <row r="41" spans="2:15">
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G41" s="51"/>
-      <c r="I41" s="30" t="s">
+      <c r="I41" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J41" s="32" t="str">
+      <c r="J41" s="31" t="str">
         <f>IF(LEFT(J40,1)="D",
       CHAR(CODE(LEFT(J40,1)) + 1)&amp;MID(J40,2,99),
       J40)</f>
         <v>E7</v>
       </c>
-      <c r="K41" s="32" t="str">
+      <c r="K41" s="31" t="str">
         <f>IF(LEFT(K40,1)="D",
       CHAR(CODE(LEFT(K40,1)) + 1)&amp;MID(K40,2,99),
       K40)</f>
         <v>E7</v>
       </c>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G42" s="52"/>
-      <c r="I42" s="30" t="s">
+      <c r="I42" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J42" s="32" t="str" cm="1">
+      <c r="J42" s="31" t="str" cm="1">
         <f t="array" aca="1" ref="J42" ca="1">IF(LEFT(J40,1)="D",
-    IF(J39=INDIRECT(J41), "with and without cache", "with cache"),
+    IF(J39=INDIRECT(J41), "normal and incognito", "normal"),
  IF(LEFT(J40,1)="E",
-        "without cache", "Incorrect cache location"
+        "incognito", "Incorrect cache location"
     )
 )</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K42" s="32" t="str" cm="1">
+        <v>normal and incognito</v>
+      </c>
+      <c r="K42" s="31" t="str" cm="1">
         <f t="array" aca="1" ref="K42" ca="1">IF(LEFT(K40,1)="D",
-    IF(K39=INDIRECT(K41), "with and without cache", "with cache"),
+    IF(K39=INDIRECT(K41), "normal and incognito", "normal"),
  IF(LEFT(K40,1)="E",
-        "without cache", "Incorrect cache location"
+        "incognito", "Incorrect cache location"
     )
 )</f>
-        <v>with and without cache</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15">
-      <c r="I43" s="30" t="s">
+        <v>normal and incognito</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I43" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J43" s="32" t="str">
+      <c r="J43" s="31" t="str">
         <f>IF(LEFT(J40,1)="D",
     CHAR(CODE(LEFT(J40,1)) - 1) &amp; MID(J40,2,99),
     CHAR(CODE(LEFT(J40,1)) - 2) &amp; MID(J40,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="K43" s="32" t="str">
+      <c r="K43" s="31" t="str">
         <f>IF(LEFT(K40,1)="D",
     CHAR(CODE(LEFT(K40,1)) - 1) &amp; MID(K40,2,99),
     CHAR(CODE(LEFT(K40,1)) - 2) &amp; MID(K40,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="L43" s="34"/>
-      <c r="M43" s="34"/>
-      <c r="N43" s="34"/>
-      <c r="O43" s="34"/>
-    </row>
-    <row r="44" spans="2:15">
-      <c r="I44" s="30" t="s">
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I44" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="J44" s="32" t="str">
+      <c r="J44" s="31" t="str">
         <f>CHAR(CODE(LEFT(J40,1))
       - IF(LEFT(J40,1)="E", 3,
            IF(LEFT(J40,1)="D", 2, 0)
@@ -2953,7 +2946,7 @@
 )</f>
         <v>B7</v>
       </c>
-      <c r="K44" s="32" t="str">
+      <c r="K44" s="31" t="str">
         <f>CHAR(CODE(LEFT(K40,1))
       - IF(LEFT(K40,1)="E", 3,
            IF(LEFT(K40,1)="D", 2, 0)
@@ -2967,48 +2960,48 @@
         <v>B6</v>
       </c>
     </row>
-    <row r="45" spans="2:15">
-      <c r="I45" s="30" t="s">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I45" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="J45" s="32" t="str" cm="1">
+      <c r="J45" s="31" t="str" cm="1">
         <f t="array" aca="1" ref="J45" ca="1">INDIRECT(J44)</f>
         <v>01_url</v>
       </c>
-      <c r="K45" s="32" cm="1">
+      <c r="K45" s="31" cm="1">
         <f t="array" aca="1" ref="K45" ca="1">INDIRECT(K44)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
-      <c r="I46" s="30" t="s">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I46" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="J46" s="32" t="str">
+      <c r="J46" s="31" t="str">
         <f ca="1">RIGHT(J47, LEN(J47) - 3)</f>
         <v>url</v>
       </c>
-      <c r="K46" s="32" t="e">
+      <c r="K46" s="31" t="e">
         <f ca="1">RIGHT(K47, LEN(K47) - 3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
-      <c r="J47" s="31" t="str" cm="1">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J47" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J47" ca="1">INDIRECT(J48)</f>
         <v>01_url</v>
       </c>
-      <c r="K47" s="31" cm="1">
+      <c r="K47" s="30" cm="1">
         <f t="array" aca="1" ref="K47" ca="1">INDIRECT(K48)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
-      <c r="J48" s="31" t="str" cm="1">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J48" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J48" ca="1">LEFT(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0)-1)&amp;(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44))-(MOD(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44)),2)=0))</f>
         <v>B7</v>
       </c>
-      <c r="K48" s="31" t="str" cm="1">
+      <c r="K48" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="K48" ca="1">LEFT(K44,MATCH(TRUE,ISNUMBER(MID(K44,ROW(INDIRECT("1:"&amp;LEN(K44))),1)+0),0)-1)&amp;(MID(K44,MATCH(TRUE,ISNUMBER(MID(K44,ROW(INDIRECT("1:"&amp;LEN(K44))),1)+0),0),LEN(K44))-(MOD(MID(K44,MATCH(TRUE,ISNUMBER(MID(K44,ROW(INDIRECT("1:"&amp;LEN(K44))),1)+0),0),LEN(K44)),2)=0))</f>
         <v>B5</v>
       </c>
@@ -3037,66 +3030,66 @@
     <mergeCell ref="B35:B36"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E8">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:E12">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:E16">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:E20">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:E24">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:E28">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:E32">
-    <cfRule type="cellIs" dxfId="3" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:E36">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3111,155 +3104,155 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B7</f>
         <v>01_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="29" spans="2:5" ht="14.45" customHeight="1"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="29" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C26:E26"/>
@@ -3287,168 +3280,168 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B11</f>
         <v>02_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="C30" s="26"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3477,165 +3470,165 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5546875" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B15</f>
         <v>03_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3664,153 +3657,153 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B19</f>
         <v>04_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3839,156 +3832,156 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.7109375" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.6640625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B23</f>
         <v>05_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="C29" s="26"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4017,161 +4010,161 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B27</f>
         <v>06_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4200,152 +4193,152 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B31</f>
         <v>07_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="44"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="43"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="45"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="47"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="45"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="44"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4373,152 +4366,152 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5546875" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B35</f>
         <v>08_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="48"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="47"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4789,13 +4782,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: add image scaling for screenshots and externalize key paths for user config (#10)
- Installed image-size for screenshot scaling
- Updated excel-template.xlsx with new formatting
- Refactored excel-writer-util to support image scaling
- Created text-writer-util to separate text writing logic
- Relocated text report name, Excel template path, and Excel output name to lighthouse.config.ts
- Updated report-path-util to use externalized text report name
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cheqteams-my.sharepoint.com/personal/vwlabajo_cheqsystems_com/Documents/Documents/Team - Performance Testing/PT - Documentation/CheQ Website Production Page Speed Insight/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85A7CDF9-1448-41CA-8A15-D50BB63BA09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{8EA300FF-E831-4373-BB35-1174E74F1E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{573A2E2B-B5CE-41B0-B334-BA4A05AE6729}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C37E2E45-7E9A-43D5-A28B-C770F3703849}"/>
   </bookViews>
@@ -28,35 +28,24 @@
     <definedName name="performanceRange" localSheetId="0">Summary!$L$6:$L$35</definedName>
     <definedName name="performanceValueRange" comment="This variable refers to the performance of all pages, for devices, cache, and without cache.">Summary!$L$6,Summary!$L$7,Summary!$L$10,Summary!$L$11,Summary!$L$14,Summary!$L$15,Summary!$L$18,Summary!$L$19,Summary!$L$22,Summary!$L$23,Summary!$L$26,Summary!$L$27,Summary!$L$30,Summary!$L$31</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -73,10 +62,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="47">
   <si>
-    <t>PageSpeed Insights</t>
+    <t>Lighthouse Insights</t>
   </si>
   <si>
-    <t>Production</t>
+    <t>URLs</t>
   </si>
   <si>
     <t xml:space="preserve">Performance </t>
@@ -88,10 +77,10 @@
     <t>Device</t>
   </si>
   <si>
-    <t>With Cache</t>
+    <t>Normal</t>
   </si>
   <si>
-    <t>Without Cache</t>
+    <t>Incognito</t>
   </si>
   <si>
     <t>Best</t>
@@ -106,10 +95,10 @@
     <t>Device Selector</t>
   </si>
   <si>
-    <t>Cell with Highest</t>
+    <t>Cell normal Highest</t>
   </si>
   <si>
-    <t>Cell with Lowest</t>
+    <t>Cell normal Lowest</t>
   </si>
   <si>
     <t>Device:</t>
@@ -175,7 +164,7 @@
     <t>Record performance value location:</t>
   </si>
   <si>
-    <t>With and Without Cache Value Location:</t>
+    <t>normal and incognito Value Location:</t>
   </si>
   <si>
     <t>Cache Value:</t>
@@ -222,7 +211,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,12 +283,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -313,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE02B2B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,9 +704,6 @@
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -727,31 +713,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -773,10 +759,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,74 +781,80 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="5" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -887,13 +879,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -902,9 +894,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -926,8 +915,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -946,8 +935,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -966,8 +955,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -986,8 +975,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1006,8 +995,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1026,8 +1015,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1046,8 +1035,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1066,8 +1055,8 @@
         <color theme="0"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFE02B2B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1075,6 +1064,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE02B2B"/>
+      <color rgb="FFFF2424"/>
+      <color rgb="FFFF4545"/>
+      <color rgb="FFDE5757"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFFF5050"/>
     </mruColors>
@@ -1828,35 +1821,35 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="101.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="33.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="31" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" style="31" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" style="31" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="31" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="31" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" style="31" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="101.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="33.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="24.88671875" style="30" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="31.33203125" style="30" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" style="30" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" style="30" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" style="30" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" style="30" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1"/>
-    <row r="2" spans="1:15" ht="15" thickBot="1">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D2" s="55" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="56"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1">
-      <c r="A3" s="4"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
       <c r="B3" s="57" t="s">
         <v>1</v>
       </c>
@@ -1865,36 +1858,36 @@
         <v>2</v>
       </c>
       <c r="E3" s="60"/>
-      <c r="F3" s="6"/>
-      <c r="J3" s="42"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1">
-      <c r="B4" s="8" t="s">
+      <c r="F3" s="5"/>
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="J5" s="35" t="s">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="J5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M5" t="s">
@@ -1907,896 +1900,896 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="6"/>
+    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J6&amp;" devices "&amp; J7 &amp;",  at  "&amp; L6
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K6 &amp;" devices "&amp; K7 &amp;", at "&amp;L7
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B7&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 01_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="36" t="str" cm="1">
+      <c r="J6" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT(M6)</f>
         <v>Desktop</v>
       </c>
-      <c r="K6" s="38" t="str" cm="1">
+      <c r="K6" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">INDIRECT(M7)</f>
         <v>Desktop</v>
       </c>
-      <c r="L6" s="40">
+      <c r="L6" s="39">
         <f>MAX(D7:E8)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="31" t="str">
+      <c r="M6" s="30" t="str">
         <f>IF(LEFT(N6,1)="D",
     CHAR(CODE(LEFT(N6,1)) - 1) &amp; MID(N6,2,99),
     CHAR(CODE(LEFT(N6,1)) - 2) &amp; MID(N6,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="N6" s="34" t="str" cm="1">
+      <c r="N6" s="33" t="str" cm="1">
         <f t="array" ref="N6">ADDRESS(MIN(IF(D7:E8=L6,ROW(D7:E8))), MIN(IF(D7:E8=L6,COLUMN(D7:E8))), 4)</f>
         <v>D7</v>
       </c>
-      <c r="O6" s="34" t="str" cm="1">
+      <c r="O6" s="33" t="str" cm="1">
         <f t="array" ref="O6">ADDRESS(MIN(IF(D7:E8=L7,ROW(D7:E8))), MIN(IF(D7:E8=L7,COLUMN(D7:E8))), 4)</f>
         <v>D7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="6"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="51"/>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="36" t="str">
-        <f ca="1">IF(J6="Desktop",IF(D7=E7,"with and without cache",(IF(D7&gt;E7,"with cache","without cache"))),IF(D8=E8,"with and without cache",(IF(D8&gt;E8,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K7" s="38" t="str">
-        <f ca="1">IF(K6="Desktop",IF(D7=E7,"with and without cache",IF(D7&lt;E7,"with cache","without cache")),IF(D8=E8,"with and without cache",IF(D8&lt;E8,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L7" s="39">
+      <c r="J7" s="35" t="str">
+        <f ca="1">IF(J6="Desktop",IF(D7=E7,"normal and incognito",(IF(D7&gt;E7,"normal","incognito"))),IF(D8=E8,"normal and incognito",(IF(D8&gt;E8,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K7" s="37" t="str">
+        <f ca="1">IF(K6="Desktop",IF(D7=E7,"normal and incognito",IF(D7&lt;E7,"normal","incognito")),IF(D8=E8,"normal and incognito",IF(D8&lt;E8,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L7" s="38">
         <f>MIN(D7:E8)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="34" t="str">
+      <c r="M7" s="33" t="str">
         <f>IF(LEFT(O6,1)="D",
     CHAR(CODE(LEFT(O6,1)) - 1) &amp; MID(O6,2,99),
     CHAR(CODE(LEFT(O6,1)) - 2) &amp; MID(O6,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-    </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1">
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+    </row>
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="54"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="6"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="52"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="L9" s="30" t="s">
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="L9" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="6"/>
+    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J10&amp;" devices "&amp; J11 &amp;",  at  "&amp; L10
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K10 &amp;" devices "&amp; K11 &amp;", at "&amp;L11
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B11&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 02_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="36" t="str" cm="1">
+      <c r="J10" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT(M10)</f>
         <v>Desktop</v>
       </c>
-      <c r="K10" s="38" t="str" cm="1">
+      <c r="K10" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">INDIRECT(M11)</f>
         <v>Desktop</v>
       </c>
-      <c r="L10" s="40">
+      <c r="L10" s="39">
         <f>MAX(D11:E12)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="31" t="str">
+      <c r="M10" s="30" t="str">
         <f>IF(LEFT(N10,1)="D",
     CHAR(CODE(LEFT(N10,1)) - 1) &amp; MID(N10,2,99),
     CHAR(CODE(LEFT(N10,1)) - 2) &amp; MID(N10,2,99)
 )</f>
         <v>C11</v>
       </c>
-      <c r="N10" s="34" t="str" cm="1">
+      <c r="N10" s="33" t="str" cm="1">
         <f t="array" ref="N10">ADDRESS(MIN(IF(D11:E12=L10,ROW(D11:E12))), MIN(IF(D11:E12=L10,COLUMN(D11:E12))), 4)</f>
         <v>D11</v>
       </c>
-      <c r="O10" s="34" t="str" cm="1">
+      <c r="O10" s="33" t="str" cm="1">
         <f t="array" ref="O10">ADDRESS(MIN(IF(D11:E12=L11,ROW(D11:E12))), MIN(IF(D11:E12=L11,COLUMN(D11:E12))), 4)</f>
         <v>D11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1">
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
       <c r="G11" s="51"/>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="36" t="str">
-        <f ca="1">IF(J10="Desktop",IF(D11=E11,"with and without cache",(IF(D11&gt;E11,"with cache","without cache"))),IF(D12=E12,"with and without cache",(IF(D12&gt;E12,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K11" s="38" t="str">
-        <f ca="1">IF(K10="Desktop",IF(D11=E11,"with and without cache",IF(D11&lt;E11,"with cache","without cache")),IF(D12=E12,"with and without cache",IF(D12&lt;E12,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L11" s="39">
+      <c r="J11" s="35" t="str">
+        <f ca="1">IF(J10="Desktop",IF(D11=E11,"normal and incognito",(IF(D11&gt;E11,"normal","incognito"))),IF(D12=E12,"normal and incognito",(IF(D12&gt;E12,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K11" s="37" t="str">
+        <f ca="1">IF(K10="Desktop",IF(D11=E11,"normal and incognito",IF(D11&lt;E11,"normal","incognito")),IF(D12=E12,"normal and incognito",IF(D12&lt;E12,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L11" s="38">
         <f>MIN(D11:E12)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="34" t="str">
+      <c r="M11" s="33" t="str">
         <f>IF(LEFT(O10,1)="D",
     CHAR(CODE(LEFT(O10,1)) - 1) &amp; MID(O10,2,99),
     CHAR(CODE(LEFT(O10,1)) - 2) &amp; MID(O10,2,99)
 )</f>
         <v>C11</v>
       </c>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-    </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1">
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="54"/>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="52"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-    </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="L13" s="30" t="s">
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+    </row>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="L13" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="6"/>
+    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J14&amp;" devices "&amp; J15 &amp;",  at  "&amp; L14
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K14 &amp;" devices "&amp; K15 &amp;", at "&amp;L15
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B15&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 03_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="36" t="str" cm="1">
+      <c r="J14" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT(M14)</f>
         <v>Desktop</v>
       </c>
-      <c r="K14" s="38" t="str" cm="1">
+      <c r="K14" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K14" ca="1">INDIRECT(M15)</f>
         <v>Desktop</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="39">
         <f>MAX(D15:E16)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="31" t="str">
+      <c r="M14" s="30" t="str">
         <f>IF(LEFT(N14,1)="D",
     CHAR(CODE(LEFT(N14,1)) - 1) &amp; MID(N14,2,99),
     CHAR(CODE(LEFT(N14,1)) - 2) &amp; MID(N14,2,99)
 )</f>
         <v>C15</v>
       </c>
-      <c r="N14" s="34" t="str" cm="1">
+      <c r="N14" s="33" t="str" cm="1">
         <f t="array" ref="N14">ADDRESS(MIN(IF(D15:E16=L14,ROW(D15:E16))), MIN(IF(D15:E16=L14,COLUMN(D15:E16))), 4)</f>
         <v>D15</v>
       </c>
-      <c r="O14" s="34" t="str" cm="1">
+      <c r="O14" s="33" t="str" cm="1">
         <f t="array" ref="O14">ADDRESS(MIN(IF(D15:E16=L15,ROW(D15:E16))), MIN(IF(D15:E16=L15,COLUMN(D15:E16))), 4)</f>
         <v>D15</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="6"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="51"/>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="36" t="str">
-        <f ca="1">IF(J14="Desktop",IF(D15=E15,"with and without cache",(IF(D15&gt;E15,"with cache","without cache"))),IF(D16=E16,"with and without cache",(IF(D16&gt;E16,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K15" s="38" t="str">
-        <f ca="1">IF(K14="Desktop",IF(D15=E15,"with and without cache",IF(D15&lt;E15,"with cache","without cache")),IF(D16=E16,"with and without cache",IF(D16&lt;E16,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L15" s="39">
+      <c r="J15" s="35" t="str">
+        <f ca="1">IF(J14="Desktop",IF(D15=E15,"normal and incognito",(IF(D15&gt;E15,"normal","incognito"))),IF(D16=E16,"normal and incognito",(IF(D16&gt;E16,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K15" s="37" t="str">
+        <f ca="1">IF(K14="Desktop",IF(D15=E15,"normal and incognito",IF(D15&lt;E15,"normal","incognito")),IF(D16=E16,"normal and incognito",IF(D16&lt;E16,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L15" s="38">
         <f>MIN(D15:E16)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="34" t="str">
+      <c r="M15" s="33" t="str">
         <f>IF(LEFT(O14,1)="D",
     CHAR(CODE(LEFT(O14,1)) - 1) &amp; MID(O14,2,99),
     CHAR(CODE(LEFT(O14,1)) - 2) &amp; MID(O14,2,99)
 )</f>
         <v>C15</v>
       </c>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1">
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="54"/>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="6"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="52"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-    </row>
-    <row r="17" spans="2:15" ht="15" thickBot="1">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="L17" s="30" t="s">
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+    </row>
+    <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="L17" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="6"/>
+    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J18&amp;" devices "&amp; J19 &amp;",  at  "&amp; L18
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K18 &amp;" devices "&amp; K19 &amp;", at "&amp;L19
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B19&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 04_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="36" t="str" cm="1">
+      <c r="J18" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">INDIRECT(M18)</f>
         <v>Desktop</v>
       </c>
-      <c r="K18" s="38" t="str" cm="1">
+      <c r="K18" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K18" ca="1">INDIRECT(M19)</f>
         <v>Desktop</v>
       </c>
-      <c r="L18" s="40">
+      <c r="L18" s="39">
         <f>MAX(D19:E20)</f>
         <v>0</v>
       </c>
-      <c r="M18" s="31" t="str">
+      <c r="M18" s="30" t="str">
         <f>IF(LEFT(N18,1)="D",
     CHAR(CODE(LEFT(N18,1)) - 1) &amp; MID(N18,2,99),
     CHAR(CODE(LEFT(N18,1)) - 2) &amp; MID(N18,2,99)
 )</f>
         <v>C19</v>
       </c>
-      <c r="N18" s="34" t="str" cm="1">
+      <c r="N18" s="33" t="str" cm="1">
         <f t="array" ref="N18">ADDRESS(MIN(IF(D19:E20=L18,ROW(D19:E20))), MIN(IF(D19:E20=L18,COLUMN(D19:E20))), 4)</f>
         <v>D19</v>
       </c>
-      <c r="O18" s="34" t="str" cm="1">
+      <c r="O18" s="33" t="str" cm="1">
         <f t="array" ref="O18">ADDRESS(MIN(IF(D19:E20=L19,ROW(D19:E20))), MIN(IF(D19:E20=L19,COLUMN(D19:E20))), 4)</f>
         <v>D19</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15" thickBot="1">
+    <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="6"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="51"/>
-      <c r="I19" s="30" t="s">
+      <c r="I19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="36" t="str">
-        <f ca="1">IF(J18="Desktop",IF(D19=E19,"with and without cache",(IF(D19&gt;E19,"with cache","without cache"))),IF(D20=E20,"with and without cache",(IF(D20&gt;E20,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K19" s="38" t="str">
-        <f ca="1">IF(K18="Desktop",IF(D19=E19,"with and without cache",IF(D19&lt;E19,"with cache","without cache")),IF(D20=E20,"with and without cache",IF(D20&lt;E20,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L19" s="39">
+      <c r="J19" s="35" t="str">
+        <f ca="1">IF(J18="Desktop",IF(D19=E19,"normal and incognito",(IF(D19&gt;E19,"normal","incognito"))),IF(D20=E20,"normal and incognito",(IF(D20&gt;E20,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K19" s="37" t="str">
+        <f ca="1">IF(K18="Desktop",IF(D19=E19,"normal and incognito",IF(D19&lt;E19,"normal","incognito")),IF(D20=E20,"normal and incognito",IF(D20&lt;E20,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L19" s="38">
         <f>MIN(D19:E20)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="34" t="str">
+      <c r="M19" s="33" t="str">
         <f>IF(LEFT(O18,1)="D",
     CHAR(CODE(LEFT(O18,1)) - 1) &amp; MID(O18,2,99),
     CHAR(CODE(LEFT(O18,1)) - 2) &amp; MID(O18,2,99)
 )</f>
         <v>C19</v>
       </c>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-    </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1">
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+    </row>
+    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="54"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="6"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="52"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-    </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="L21" s="30" t="s">
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+    </row>
+    <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="L21" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
     </row>
-    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="6"/>
+    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J22&amp;" devices "&amp; J23 &amp;",  at  "&amp; L22
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K22 &amp;" devices "&amp; K23 &amp;", at "&amp;L23
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B23&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 05_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I22" s="30" t="s">
+      <c r="I22" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="36" t="str" cm="1">
+      <c r="J22" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">INDIRECT(M22)</f>
         <v>Desktop</v>
       </c>
-      <c r="K22" s="38" t="str" cm="1">
+      <c r="K22" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K22" ca="1">INDIRECT(M23)</f>
         <v>Desktop</v>
       </c>
-      <c r="L22" s="40">
+      <c r="L22" s="39">
         <f>MAX(D23:E24)</f>
         <v>0</v>
       </c>
-      <c r="M22" s="31" t="str">
+      <c r="M22" s="30" t="str">
         <f>IF(LEFT(N22,1)="D",
     CHAR(CODE(LEFT(N22,1)) - 1) &amp; MID(N22,2,99),
     CHAR(CODE(LEFT(N22,1)) - 2) &amp; MID(N22,2,99)
 )</f>
         <v>C23</v>
       </c>
-      <c r="N22" s="34" t="str" cm="1">
+      <c r="N22" s="33" t="str" cm="1">
         <f t="array" ref="N22">ADDRESS(MIN(IF(D23:E24=L22,ROW(D23:E24))), MIN(IF(D23:E24=L22,COLUMN(D23:E24))), 4)</f>
         <v>D23</v>
       </c>
-      <c r="O22" s="34" t="str" cm="1">
+      <c r="O22" s="33" t="str" cm="1">
         <f t="array" ref="O22">ADDRESS(MIN(IF(D23:E24=L23,ROW(D23:E24))), MIN(IF(D23:E24=L23,COLUMN(D23:E24))), 4)</f>
         <v>D23</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="15" thickBot="1">
+    <row r="23" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="6"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="51"/>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="36" t="str">
-        <f ca="1">IF(J22="Desktop",IF(D23=E23,"with and without cache",(IF(D23&gt;E23,"with cache","without cache"))),IF(D24=E24,"with and without cache",(IF(D24&gt;E24,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K23" s="38" t="str">
-        <f ca="1">IF(K22="Desktop",IF(D23=E23,"with and without cache",IF(D23&lt;E23,"with cache","without cache")),IF(D24=E24,"with and without cache",IF(D24&lt;E24,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L23" s="39">
+      <c r="J23" s="35" t="str">
+        <f ca="1">IF(J22="Desktop",IF(D23=E23,"normal and incognito",(IF(D23&gt;E23,"normal","incognito"))),IF(D24=E24,"normal and incognito",(IF(D24&gt;E24,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K23" s="37" t="str">
+        <f ca="1">IF(K22="Desktop",IF(D23=E23,"normal and incognito",IF(D23&lt;E23,"normal","incognito")),IF(D24=E24,"normal and incognito",IF(D24&lt;E24,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L23" s="38">
         <f>MIN(D23:E24)</f>
         <v>0</v>
       </c>
-      <c r="M23" s="34" t="str">
+      <c r="M23" s="33" t="str">
         <f>IF(LEFT(O22,1)="D",
     CHAR(CODE(LEFT(O22,1)) - 1) &amp; MID(O22,2,99),
     CHAR(CODE(LEFT(O22,1)) - 2) &amp; MID(O22,2,99)
 )</f>
         <v>C23</v>
       </c>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-    </row>
-    <row r="24" spans="2:15" ht="15" thickBot="1">
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+    </row>
+    <row r="24" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="54"/>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="6"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="52"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-    </row>
-    <row r="25" spans="2:15" ht="15" thickBot="1">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="L25" s="30" t="s">
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+    </row>
+    <row r="25" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="L25" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
     </row>
-    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="6"/>
+    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J26&amp;" devices "&amp; J27 &amp;",  at  "&amp; L26
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K26 &amp;" devices "&amp; K27 &amp;", at "&amp;L27
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B27&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 06_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="36" t="str" cm="1">
+      <c r="J26" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J26" ca="1">INDIRECT(M26)</f>
         <v>Desktop</v>
       </c>
-      <c r="K26" s="38" t="str" cm="1">
+      <c r="K26" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K26" ca="1">INDIRECT(M27)</f>
         <v>Desktop</v>
       </c>
-      <c r="L26" s="40">
+      <c r="L26" s="39">
         <f>MAX(D27:E28)</f>
         <v>0</v>
       </c>
-      <c r="M26" s="31" t="str">
+      <c r="M26" s="30" t="str">
         <f>IF(LEFT(N26,1)="D",
     CHAR(CODE(LEFT(N26,1)) - 1) &amp; MID(N26,2,99),
     CHAR(CODE(LEFT(N26,1)) - 2) &amp; MID(N26,2,99)
 )</f>
         <v>C27</v>
       </c>
-      <c r="N26" s="34" t="str" cm="1">
+      <c r="N26" s="33" t="str" cm="1">
         <f t="array" ref="N26">ADDRESS(MIN(IF(D27:E28=L26,ROW(D27:E28))), MIN(IF(D27:E28=L26,COLUMN(D27:E28))), 4)</f>
         <v>D27</v>
       </c>
-      <c r="O26" s="34" t="str" cm="1">
+      <c r="O26" s="33" t="str" cm="1">
         <f t="array" ref="O26">ADDRESS(MIN(IF(D27:E28=L27,ROW(D27:E28))), MIN(IF(D27:E28=L27,COLUMN(D27:E28))), 4)</f>
         <v>D27</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="15" thickBot="1">
+    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="6"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="51"/>
-      <c r="I27" s="30" t="s">
+      <c r="I27" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J27" s="36" t="str">
-        <f ca="1">IF(J26="Desktop",IF(D27=E27,"with and without cache",(IF(D27&gt;E27,"with cache","without cache"))),IF(D28=E28,"with and without cache",(IF(D28&gt;E28,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K27" s="38" t="str">
-        <f ca="1">IF(K26="Desktop",IF(D27=E27,"with and without cache",IF(D27&lt;E27,"with cache","without cache")),IF(D28=E28,"with and without cache",IF(D28&lt;E28,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L27" s="39">
+      <c r="J27" s="35" t="str">
+        <f ca="1">IF(J26="Desktop",IF(D27=E27,"normal and incognito",(IF(D27&gt;E27,"normal","incognito"))),IF(D28=E28,"normal and incognito",(IF(D28&gt;E28,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K27" s="37" t="str">
+        <f ca="1">IF(K26="Desktop",IF(D27=E27,"normal and incognito",IF(D27&lt;E27,"normal","incognito")),IF(D28=E28,"normal and incognito",IF(D28&lt;E28,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L27" s="38">
         <f>MIN(D27:E28)</f>
         <v>0</v>
       </c>
-      <c r="M27" s="34" t="str">
+      <c r="M27" s="33" t="str">
         <f>IF(LEFT(O26,1)="D",
     CHAR(CODE(LEFT(O26,1)) - 1) &amp; MID(O26,2,99),
     CHAR(CODE(LEFT(O26,1)) - 2) &amp; MID(O26,2,99)
 )</f>
         <v>C27</v>
       </c>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-    </row>
-    <row r="28" spans="2:15" ht="15" thickBot="1">
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="54"/>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="6"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="52"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-    </row>
-    <row r="29" spans="2:15" ht="15" thickBot="1">
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="L29" s="30" t="s">
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+    </row>
+    <row r="29" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="L29" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
     </row>
-    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="6"/>
+    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J30&amp;" devices "&amp; J31 &amp;",  at  "&amp; L30
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K30 &amp;" devices "&amp; K31 &amp;", at "&amp;L31
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B31&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 07_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I30" s="30" t="s">
+      <c r="I30" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J30" s="36" t="str" cm="1">
+      <c r="J30" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J30" ca="1">INDIRECT(M30)</f>
         <v>Desktop</v>
       </c>
-      <c r="K30" s="38" t="str" cm="1">
+      <c r="K30" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K30" ca="1">INDIRECT(M31)</f>
         <v>Desktop</v>
       </c>
-      <c r="L30" s="40">
+      <c r="L30" s="39">
         <f>MAX(D31:E32)</f>
         <v>0</v>
       </c>
-      <c r="M30" s="31" t="str">
+      <c r="M30" s="30" t="str">
         <f>IF(LEFT(N30,1)="D",
     CHAR(CODE(LEFT(N30,1)) - 1) &amp; MID(N30,2,99),
     CHAR(CODE(LEFT(N30,1)) - 2) &amp; MID(N30,2,99)
 )</f>
         <v>C31</v>
       </c>
-      <c r="N30" s="34" t="str" cm="1">
+      <c r="N30" s="33" t="str" cm="1">
         <f t="array" ref="N30">ADDRESS(MIN(IF(D31:E32=L30,ROW(D31:E32))), MIN(IF(D31:E32=L30,COLUMN(D31:E32))), 4)</f>
         <v>D31</v>
       </c>
-      <c r="O30" s="34" t="str" cm="1">
+      <c r="O30" s="33" t="str" cm="1">
         <f t="array" ref="O30">ADDRESS(MIN(IF(D31:E32=L31,ROW(D31:E32))), MIN(IF(D31:E32=L31,COLUMN(D31:E32))), 4)</f>
         <v>D31</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="15" thickBot="1">
+    <row r="31" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="6"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="51"/>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="36" t="str">
-        <f ca="1">IF(J30="Desktop",IF(D31=E31,"with and without cache",(IF(D31&gt;E31,"with cache","without cache"))),IF(D32=E32,"with and without cache",(IF(D32&gt;E32,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K31" s="38" t="str">
-        <f ca="1">IF(K30="Desktop",IF(D31=E31,"with and without cache",IF(D31&lt;E31,"with cache","without cache")),IF(D32=E32,"with and without cache",IF(D32&lt;E32,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L31" s="39">
+      <c r="J31" s="35" t="str">
+        <f ca="1">IF(J30="Desktop",IF(D31=E31,"normal and incognito",(IF(D31&gt;E31,"normal","incognito"))),IF(D32=E32,"normal and incognito",(IF(D32&gt;E32,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K31" s="37" t="str">
+        <f ca="1">IF(K30="Desktop",IF(D31=E31,"normal and incognito",IF(D31&lt;E31,"normal","incognito")),IF(D32=E32,"normal and incognito",IF(D32&lt;E32,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L31" s="38">
         <f>MIN(D31:E32)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="34" t="str">
+      <c r="M31" s="33" t="str">
         <f>IF(LEFT(O30,1)="D",
     CHAR(CODE(LEFT(O30,1)) - 1) &amp; MID(O30,2,99),
     CHAR(CODE(LEFT(O30,1)) - 2) &amp; MID(O30,2,99)
 )</f>
         <v>C31</v>
       </c>
-      <c r="N31" s="34"/>
-      <c r="O31" s="34"/>
-    </row>
-    <row r="32" spans="2:15">
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="54"/>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="6"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="52"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-    </row>
-    <row r="33" spans="2:15">
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="43"/>
-      <c r="L33" s="30" t="s">
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="42"/>
+      <c r="L33" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M33"/>
       <c r="N33"/>
       <c r="O33"/>
     </row>
-    <row r="34" spans="2:15" ht="14.45" customHeight="1">
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="6"/>
+    <row r="34" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="50" t="str">
         <f ca="1">"The best recorded performance score was in "&amp;J34&amp;" devices "&amp; J35 &amp;",  at  "&amp; L34
 &amp;CHAR(10)&amp;
 "The worst recorded performance score was in "&amp; K34 &amp;" devices "&amp; K35 &amp;", at "&amp;L35
 &amp;CHAR(10)&amp;
 "Refer to "&amp;B35&amp;" tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>The best recorded performance score was in Desktop devices with and without cache,  at  0
-The worst recorded performance score was in Desktop devices with and without cache, at 0
+        <v>The best recorded performance score was in Desktop devices normal and incognito,  at  0
+The worst recorded performance score was in Desktop devices normal and incognito, at 0
 Refer to 08_url tab for the best and worst insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
-      <c r="I34" s="30" t="s">
+      <c r="I34" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J34" s="36" t="str" cm="1">
+      <c r="J34" s="35" t="str" cm="1">
         <f t="array" aca="1" ref="J34" ca="1">INDIRECT(M34)</f>
         <v>Desktop</v>
       </c>
-      <c r="K34" s="38" t="str" cm="1">
+      <c r="K34" s="37" t="str" cm="1">
         <f t="array" aca="1" ref="K34" ca="1">INDIRECT(M35)</f>
         <v>Desktop</v>
       </c>
-      <c r="L34" s="40">
+      <c r="L34" s="39">
         <f>MAX(D35:E36)</f>
         <v>0</v>
       </c>
-      <c r="M34" s="31" t="str">
+      <c r="M34" s="30" t="str">
         <f>IF(LEFT(N34,1)="D",
     CHAR(CODE(LEFT(N34,1)) - 1) &amp; MID(N34,2,99),
     CHAR(CODE(LEFT(N34,1)) - 2) &amp; MID(N34,2,99)
 )</f>
         <v>C35</v>
       </c>
-      <c r="N34" s="34" t="str" cm="1">
+      <c r="N34" s="33" t="str" cm="1">
         <f t="array" ref="N34">ADDRESS(MIN(IF(D35:E36=L34,ROW(D35:E36))), MIN(IF(D35:E36=L34,COLUMN(D35:E36))), 4)</f>
         <v>D35</v>
       </c>
-      <c r="O34" s="34" t="str" cm="1">
+      <c r="O34" s="33" t="str" cm="1">
         <f t="array" ref="O34">ADDRESS(MIN(IF(D35:E36=L35,ROW(D35:E36))), MIN(IF(D35:E36=L35,COLUMN(D35:E36))), 4)</f>
         <v>D35</v>
       </c>
     </row>
-    <row r="35" spans="2:15">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="6"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="51"/>
-      <c r="I35" s="30" t="s">
+      <c r="I35" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J35" s="36" t="str">
-        <f ca="1">IF(J34="Desktop",IF(D35=E35,"with and without cache",(IF(D35&gt;E35,"with cache","without cache"))),IF(D36=E36,"with and without cache",(IF(D36&gt;E36,"with cache","without cache"))))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K35" s="38" t="str">
-        <f ca="1">IF(K34="Desktop",IF(D35=E35,"with and without cache",IF(D35&lt;E35,"with cache","without cache")),IF(D36=E36,"with and without cache",IF(D36&lt;E36,"with cache","without cache")))</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="L35" s="39">
+      <c r="J35" s="35" t="str">
+        <f ca="1">IF(J34="Desktop",IF(D35=E35,"normal and incognito",(IF(D35&gt;E35,"normal","incognito"))),IF(D36=E36,"normal and incognito",(IF(D36&gt;E36,"normal","incognito"))))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="K35" s="37" t="str">
+        <f ca="1">IF(K34="Desktop",IF(D35=E35,"normal and incognito",IF(D35&lt;E35,"normal","incognito")),IF(D36=E36,"normal and incognito",IF(D36&lt;E36,"normal","incognito")))</f>
+        <v>normal and incognito</v>
+      </c>
+      <c r="L35" s="38">
         <f>MIN(D35:E36)</f>
         <v>0</v>
       </c>
-      <c r="M35" s="34" t="str">
+      <c r="M35" s="33" t="str">
         <f>IF(LEFT(O34,1)="D",
     CHAR(CODE(LEFT(O34,1)) - 1) &amp; MID(O34,2,99),
     CHAR(CODE(LEFT(O34,1)) - 2) &amp; MID(O34,2,99)
 )</f>
         <v>C35</v>
       </c>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34"/>
-    </row>
-    <row r="36" spans="2:15">
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36" s="54"/>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="6"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="52"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-    </row>
-    <row r="37" spans="2:15">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="34"/>
-    </row>
-    <row r="38" spans="2:15" ht="14.45" customHeight="1">
-      <c r="C38" s="12" t="s">
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+    </row>
+    <row r="38" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="6"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="50" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">IFERROR(
     "The best recorded performance score was in the " &amp; J46 &amp; " page for " &amp; INDIRECT(J43) &amp; " devices " &amp; J42 &amp; ", at " &amp; J39 &amp; CHAR(10) &amp;
@@ -2807,140 +2800,140 @@
 )</f>
         <v>Kindly, fill the Performance Score first!</v>
       </c>
-      <c r="I38" s="30" t="s">
+      <c r="I38" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J38" s="32" t="s">
+      <c r="J38" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K38" s="32" t="s">
+      <c r="K38" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="L38" s="34"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34"/>
-    </row>
-    <row r="39" spans="2:15">
-      <c r="C39" s="13" t="s">
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+      <c r="O38" s="33"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C39" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="6"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="51"/>
-      <c r="I39" s="30" t="s">
+      <c r="I39" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J39" s="32">
+      <c r="J39" s="31">
         <f>MAX(performanceRange)</f>
         <v>0</v>
       </c>
-      <c r="K39" s="33">
+      <c r="K39" s="32">
         <f>MIN(performanceRange)</f>
         <v>0</v>
       </c>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-    </row>
-    <row r="40" spans="2:15">
-      <c r="C40" s="14" t="s">
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C40" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="6"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="51"/>
-      <c r="I40" s="30" t="s">
+      <c r="I40" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="32" t="str" cm="1">
+      <c r="J40" s="31" t="str" cm="1">
         <f t="array" ref="J40">ADDRESS(MIN(IF(D7:E36=J39,ROW(D7:E36))), MIN(IF(D7:E36=J39,COLUMN(D7:E36))), 4)</f>
         <v>D7</v>
       </c>
-      <c r="K40" s="32" t="str" cm="1">
+      <c r="K40" s="31" t="str" cm="1">
         <f t="array" ref="K40">ADDRESS(MIN(IF(D7:E36=K39,ROW(D7:E36))), MIN(IF(D7:E36=K39,COLUMN(D7:E36))), 4)</f>
         <v>D7</v>
       </c>
-      <c r="L40" s="34"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
-      <c r="O40" s="34"/>
-    </row>
-    <row r="41" spans="2:15">
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G41" s="51"/>
-      <c r="I41" s="30" t="s">
+      <c r="I41" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J41" s="32" t="str">
+      <c r="J41" s="31" t="str">
         <f>IF(LEFT(J40,1)="D",
       CHAR(CODE(LEFT(J40,1)) + 1)&amp;MID(J40,2,99),
       J40)</f>
         <v>E7</v>
       </c>
-      <c r="K41" s="32" t="str">
+      <c r="K41" s="31" t="str">
         <f>IF(LEFT(K40,1)="D",
       CHAR(CODE(LEFT(K40,1)) + 1)&amp;MID(K40,2,99),
       K40)</f>
         <v>E7</v>
       </c>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G42" s="52"/>
-      <c r="I42" s="30" t="s">
+      <c r="I42" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J42" s="32" t="str" cm="1">
+      <c r="J42" s="31" t="str" cm="1">
         <f t="array" aca="1" ref="J42" ca="1">IF(LEFT(J40,1)="D",
-    IF(J39=INDIRECT(J41), "with and without cache", "with cache"),
+    IF(J39=INDIRECT(J41), "normal and incognito", "normal"),
  IF(LEFT(J40,1)="E",
-        "without cache", "Incorrect cache location"
+        "incognito", "Incorrect cache location"
     )
 )</f>
-        <v>with and without cache</v>
-      </c>
-      <c r="K42" s="32" t="str" cm="1">
+        <v>normal and incognito</v>
+      </c>
+      <c r="K42" s="31" t="str" cm="1">
         <f t="array" aca="1" ref="K42" ca="1">IF(LEFT(K40,1)="D",
-    IF(K39=INDIRECT(K41), "with and without cache", "with cache"),
+    IF(K39=INDIRECT(K41), "normal and incognito", "normal"),
  IF(LEFT(K40,1)="E",
-        "without cache", "Incorrect cache location"
+        "incognito", "Incorrect cache location"
     )
 )</f>
-        <v>with and without cache</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15">
-      <c r="I43" s="30" t="s">
+        <v>normal and incognito</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I43" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J43" s="32" t="str">
+      <c r="J43" s="31" t="str">
         <f>IF(LEFT(J40,1)="D",
     CHAR(CODE(LEFT(J40,1)) - 1) &amp; MID(J40,2,99),
     CHAR(CODE(LEFT(J40,1)) - 2) &amp; MID(J40,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="K43" s="32" t="str">
+      <c r="K43" s="31" t="str">
         <f>IF(LEFT(K40,1)="D",
     CHAR(CODE(LEFT(K40,1)) - 1) &amp; MID(K40,2,99),
     CHAR(CODE(LEFT(K40,1)) - 2) &amp; MID(K40,2,99)
 )</f>
         <v>C7</v>
       </c>
-      <c r="L43" s="34"/>
-      <c r="M43" s="34"/>
-      <c r="N43" s="34"/>
-      <c r="O43" s="34"/>
-    </row>
-    <row r="44" spans="2:15">
-      <c r="I44" s="30" t="s">
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I44" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="J44" s="32" t="str">
+      <c r="J44" s="31" t="str">
         <f>CHAR(CODE(LEFT(J40,1))
       - IF(LEFT(J40,1)="E", 3,
            IF(LEFT(J40,1)="D", 2, 0)
@@ -2953,7 +2946,7 @@
 )</f>
         <v>B7</v>
       </c>
-      <c r="K44" s="32" t="str">
+      <c r="K44" s="31" t="str">
         <f>CHAR(CODE(LEFT(K40,1))
       - IF(LEFT(K40,1)="E", 3,
            IF(LEFT(K40,1)="D", 2, 0)
@@ -2967,48 +2960,48 @@
         <v>B6</v>
       </c>
     </row>
-    <row r="45" spans="2:15">
-      <c r="I45" s="30" t="s">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I45" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="J45" s="32" t="str" cm="1">
+      <c r="J45" s="31" t="str" cm="1">
         <f t="array" aca="1" ref="J45" ca="1">INDIRECT(J44)</f>
         <v>01_url</v>
       </c>
-      <c r="K45" s="32" cm="1">
+      <c r="K45" s="31" cm="1">
         <f t="array" aca="1" ref="K45" ca="1">INDIRECT(K44)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
-      <c r="I46" s="30" t="s">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I46" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="J46" s="32" t="str">
+      <c r="J46" s="31" t="str">
         <f ca="1">RIGHT(J47, LEN(J47) - 3)</f>
         <v>url</v>
       </c>
-      <c r="K46" s="32" t="e">
+      <c r="K46" s="31" t="e">
         <f ca="1">RIGHT(K47, LEN(K47) - 3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
-      <c r="J47" s="31" t="str" cm="1">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J47" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J47" ca="1">INDIRECT(J48)</f>
         <v>01_url</v>
       </c>
-      <c r="K47" s="31" cm="1">
+      <c r="K47" s="30" cm="1">
         <f t="array" aca="1" ref="K47" ca="1">INDIRECT(K48)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
-      <c r="J48" s="31" t="str" cm="1">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J48" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J48" ca="1">LEFT(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0)-1)&amp;(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44))-(MOD(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44)),2)=0))</f>
         <v>B7</v>
       </c>
-      <c r="K48" s="31" t="str" cm="1">
+      <c r="K48" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="K48" ca="1">LEFT(K44,MATCH(TRUE,ISNUMBER(MID(K44,ROW(INDIRECT("1:"&amp;LEN(K44))),1)+0),0)-1)&amp;(MID(K44,MATCH(TRUE,ISNUMBER(MID(K44,ROW(INDIRECT("1:"&amp;LEN(K44))),1)+0),0),LEN(K44))-(MOD(MID(K44,MATCH(TRUE,ISNUMBER(MID(K44,ROW(INDIRECT("1:"&amp;LEN(K44))),1)+0),0),LEN(K44)),2)=0))</f>
         <v>B5</v>
       </c>
@@ -3037,66 +3030,66 @@
     <mergeCell ref="B35:B36"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E8">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:E12">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:E16">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:E20">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:E24">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:E28">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:E32">
-    <cfRule type="cellIs" dxfId="3" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:E36">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3111,155 +3104,155 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B7</f>
         <v>01_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="29" spans="2:5" ht="14.45" customHeight="1"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="29" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C26:E26"/>
@@ -3287,168 +3280,168 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B11</f>
         <v>02_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="C30" s="26"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3477,165 +3470,165 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5546875" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B15</f>
         <v>03_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3664,153 +3657,153 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B19</f>
         <v>04_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3839,156 +3832,156 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.7109375" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.6640625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B23</f>
         <v>05_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="C29" s="26"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4017,161 +4010,161 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="C2" s="61">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="64">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="66" t="str">
         <f>Summary!B27</f>
         <v>06_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4200,152 +4193,152 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B31</f>
         <v>07_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="44"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="43"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="45"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="47"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="45"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="44"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="76"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1">
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4373,152 +4366,152 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5546875" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
-      <c r="C2" s="61">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="64">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="63" t="str">
+      <c r="D2" s="65"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="str">
         <f>Summary!B35</f>
         <v>08_url</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="22" t="s">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="67"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64"/>
-      <c r="C5" s="67" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="67"/>
+      <c r="C5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="65"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="23" t="s">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="72">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D9" s="73"/>
+      <c r="E9" s="74"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="48"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="D10" s="47"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="75"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="D11" s="78"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="69">
+      <c r="C25" s="72">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4789,13 +4782,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: improve audit data handling and prepare for future spinner support
- Set screenshot option to static 1 temporarily (pending Excel writer support)
- Changed run-all-lighthouse to use static data
- Updated excel-template.xlsx
- Refactored excel-writer-util:
  • Added audit option
  • Moved diagnostic and audit data gathering to dynamic functions
  • Moved screenshot adding to a dynamic function
- Refactored lighthouse-runner-util:
  • Removed some report summary logs
  • Added audits data to text-writer-util
- Refactored screenshot-util:
  • Moved diagnostic data gathering to a separate function
  • Added and moved audit data gathering to a separate function
- Added spinner-util (not yet implemented, execSync → execAsync needed)
- Refactored text-writer-util to include audits data
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29203"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cheqteams-my.sharepoint.com/personal/vwlabajo_cheqsystems_com/Documents/Documents/Team - Performance Testing/PT - Documentation/CheQ Website Production Page Speed Insight/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8EA300FF-E831-4373-BB35-1174E74F1E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{573A2E2B-B5CE-41B0-B334-BA4A05AE6729}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2009E814-DD03-4F30-B2EF-0CCF18B8CF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C37E2E45-7E9A-43D5-A28B-C770F3703849}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C37E2E45-7E9A-43D5-A28B-C770F3703849}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,24 +28,35 @@
     <definedName name="performanceRange" localSheetId="0">Summary!$L$6:$L$35</definedName>
     <definedName name="performanceValueRange" comment="This variable refers to the performance of all pages, for devices, cache, and without cache.">Summary!$L$6,Summary!$L$7,Summary!$L$10,Summary!$L$11,Summary!$L$14,Summary!$L$15,Summary!$L$18,Summary!$L$19,Summary!$L$22,Summary!$L$23,Summary!$L$26,Summary!$L$27,Summary!$L$30,Summary!$L$31</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -60,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="45">
   <si>
     <t>Lighthouse Insights</t>
   </si>
@@ -191,13 +202,7 @@
     <t>Diagnostic:</t>
   </si>
   <si>
-    <t>Defer offscreen images</t>
-  </si>
-  <si>
     <t>Recommendation:</t>
-  </si>
-  <si>
-    <t>Learn how to defer offscreen images</t>
   </si>
   <si>
     <t>Worst Insight</t>
@@ -211,7 +216,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,12 +259,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -702,7 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -812,13 +811,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -828,12 +829,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -852,9 +847,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -894,6 +886,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1081,422 +1076,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7EB9A-6084-4497-A764-1BC71B7E8699}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2219325"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE12300-F126-4D9C-97C2-D10A8F0E5655}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2200275"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B26E2C4F-528F-4CCD-84B1-FC2BFEFFC45B}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948B4D1A-F86F-48BA-BF04-2A24804F7EAB}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EF85C6E-6393-4B76-B446-C0AB608C2980}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECEC0987-0254-40BD-8131-5086609B56A9}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EECBFD6-95BA-4D5A-B6B9-39BC356E8EF9}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2190750"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EFADFC0-E695-49D0-B5E0-865C7C62DDBD}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2190750"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1819,49 +1398,49 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="7" width="101.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="24.88671875" style="30" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" style="30" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="29.33203125" style="30" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" style="30" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" style="30" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" style="30" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="30" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" style="30" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="29.28515625" style="30" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="30" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" style="30" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" style="30" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="56"/>
+    <row r="1" spans="1:15" ht="15" thickBot="1"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1">
+      <c r="D2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="54"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="60"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="5"/>
       <c r="J3" s="41"/>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1876,7 +1455,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15" thickBot="1">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="5"/>
@@ -1900,7 +1479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="26"/>
@@ -1947,8 +1526,8 @@
         <v>D7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="53" t="s">
+    <row r="7" spans="1:15" ht="15" thickBot="1">
+      <c r="B7" s="48" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1983,8 +1562,8 @@
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
     </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="54"/>
+    <row r="8" spans="1:15" ht="15" thickBot="1">
+      <c r="B8" s="49"/>
       <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
@@ -1996,7 +1575,7 @@
       <c r="N8" s="33"/>
       <c r="O8" s="33"/>
     </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15" thickBot="1">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2010,7 +1589,7 @@
       <c r="N9"/>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="26"/>
@@ -2057,8 +1636,8 @@
         <v>D11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="53" t="s">
+    <row r="11" spans="1:15" ht="15" thickBot="1">
+      <c r="B11" s="48" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -2092,8 +1671,8 @@
       <c r="N11" s="33"/>
       <c r="O11" s="33"/>
     </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="54"/>
+    <row r="12" spans="1:15" ht="15" thickBot="1">
+      <c r="B12" s="49"/>
       <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
@@ -2106,7 +1685,7 @@
       <c r="N12" s="33"/>
       <c r="O12" s="33"/>
     </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="15" thickBot="1">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="14"/>
@@ -2120,7 +1699,7 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="26"/>
@@ -2167,8 +1746,8 @@
         <v>D15</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="53" t="s">
+    <row r="15" spans="1:15" ht="15" thickBot="1">
+      <c r="B15" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -2203,8 +1782,8 @@
       <c r="N15" s="33"/>
       <c r="O15" s="33"/>
     </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="54"/>
+    <row r="16" spans="1:15" ht="15" thickBot="1">
+      <c r="B16" s="49"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -2217,7 +1796,7 @@
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
     </row>
-    <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" ht="15" thickBot="1">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="14"/>
@@ -2231,7 +1810,7 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="26"/>
@@ -2278,8 +1857,8 @@
         <v>D19</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="53" t="s">
+    <row r="19" spans="2:15" ht="15" thickBot="1">
+      <c r="B19" s="48" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -2314,8 +1893,8 @@
       <c r="N19" s="33"/>
       <c r="O19" s="33"/>
     </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="54"/>
+    <row r="20" spans="2:15" ht="15" thickBot="1">
+      <c r="B20" s="49"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -2328,7 +1907,7 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" ht="15" thickBot="1">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="14"/>
@@ -2342,7 +1921,7 @@
       <c r="N21"/>
       <c r="O21"/>
     </row>
-    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="26"/>
@@ -2389,8 +1968,8 @@
         <v>D23</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="53" t="s">
+    <row r="23" spans="2:15" ht="15" thickBot="1">
+      <c r="B23" s="48" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -2425,8 +2004,8 @@
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
     </row>
-    <row r="24" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="54"/>
+    <row r="24" spans="2:15" ht="15" thickBot="1">
+      <c r="B24" s="49"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -2439,7 +2018,7 @@
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
     </row>
-    <row r="25" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:15" ht="15" thickBot="1">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="14"/>
@@ -2453,7 +2032,7 @@
       <c r="N25"/>
       <c r="O25"/>
     </row>
-    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="26"/>
@@ -2500,8 +2079,8 @@
         <v>D27</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="53" t="s">
+    <row r="27" spans="2:15" ht="15" thickBot="1">
+      <c r="B27" s="48" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -2536,8 +2115,8 @@
       <c r="N27" s="33"/>
       <c r="O27" s="33"/>
     </row>
-    <row r="28" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="54"/>
+    <row r="28" spans="2:15" ht="15" thickBot="1">
+      <c r="B28" s="49"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -2550,7 +2129,7 @@
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
     </row>
-    <row r="29" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:15" ht="15" thickBot="1">
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="14"/>
@@ -2564,7 +2143,7 @@
       <c r="N29"/>
       <c r="O29"/>
     </row>
-    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="26"/>
@@ -2611,8 +2190,8 @@
         <v>D31</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="53" t="s">
+    <row r="31" spans="2:15" ht="15" thickBot="1">
+      <c r="B31" s="48" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -2647,8 +2226,8 @@
       <c r="N31" s="33"/>
       <c r="O31" s="33"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="54"/>
+    <row r="32" spans="2:15">
+      <c r="B32" s="49"/>
       <c r="C32" s="10" t="s">
         <v>17</v>
       </c>
@@ -2661,7 +2240,7 @@
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15">
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="14"/>
@@ -2675,7 +2254,7 @@
       <c r="N33"/>
       <c r="O33"/>
     </row>
-    <row r="34" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" ht="14.45" customHeight="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="26"/>
@@ -2722,8 +2301,8 @@
         <v>D35</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="53" t="s">
+    <row r="35" spans="2:15">
+      <c r="B35" s="48" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -2758,8 +2337,8 @@
       <c r="N35" s="33"/>
       <c r="O35" s="33"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="54"/>
+    <row r="36" spans="2:15">
+      <c r="B36" s="49"/>
       <c r="C36" s="10" t="s">
         <v>17</v>
       </c>
@@ -2772,7 +2351,7 @@
       <c r="N36" s="33"/>
       <c r="O36" s="33"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:15">
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="F37" s="5"/>
@@ -2782,11 +2361,11 @@
       <c r="N37" s="33"/>
       <c r="O37" s="33"/>
     </row>
-    <row r="38" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" ht="14.45" customHeight="1">
       <c r="C38" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="47" t="s">
         <v>26</v>
       </c>
       <c r="F38" s="5"/>
@@ -2814,7 +2393,7 @@
       <c r="N38" s="33"/>
       <c r="O38" s="33"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:15">
       <c r="C39" s="12" t="s">
         <v>28</v>
       </c>
@@ -2839,7 +2418,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="33"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15">
       <c r="C40" s="13" t="s">
         <v>31</v>
       </c>
@@ -2864,7 +2443,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="33"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15">
       <c r="G41" s="51"/>
       <c r="I41" s="29" t="s">
         <v>34</v>
@@ -2882,7 +2461,7 @@
         <v>E7</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15">
       <c r="G42" s="52"/>
       <c r="I42" s="29" t="s">
         <v>35</v>
@@ -2906,7 +2485,7 @@
         <v>normal and incognito</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:15">
       <c r="I43" s="29" t="s">
         <v>36</v>
       </c>
@@ -2929,7 +2508,7 @@
       <c r="N43" s="33"/>
       <c r="O43" s="33"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:15">
       <c r="I44" s="29" t="s">
         <v>37</v>
       </c>
@@ -2960,7 +2539,7 @@
         <v>B6</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15">
       <c r="I45" s="29" t="s">
         <v>38</v>
       </c>
@@ -2973,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15">
       <c r="I46" s="29" t="s">
         <v>39</v>
       </c>
@@ -2986,7 +2565,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15">
       <c r="J47" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J47" ca="1">INDIRECT(J48)</f>
         <v>01_url</v>
@@ -2996,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15">
       <c r="J48" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J48" ca="1">LEFT(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0)-1)&amp;(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44))-(MOD(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44)),2)=0))</f>
         <v>B7</v>
@@ -3008,15 +2587,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="G10:G12"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="G38:G42"/>
     <mergeCell ref="B19:B20"/>
@@ -3028,68 +2598,77 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="G34:G36"/>
     <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="G10:G12"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:E8">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="D35:E36">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:E32">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:E28">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:E24">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:E20">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:E16">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:E12">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:E16">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="D7:E8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19:E20">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23:E24">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:E28">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31:E32">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="14" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:E36">
-    <cfRule type="cellIs" dxfId="1" priority="15" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3104,30 +2683,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.109375" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B7</f>
         <v>01_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3135,17 +2714,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3153,106 +2732,102 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="29" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:5" ht="14.45" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C26:E26"/>
@@ -3265,11 +2840,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{958DC036-E7D9-4E9F-92F1-E9C4EDA77823}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3280,30 +2851,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.109375" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B11</f>
         <v>02_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3311,17 +2882,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3329,118 +2900,114 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5">
       <c r="C30" s="25"/>
     </row>
   </sheetData>
@@ -3455,11 +3022,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{9D988C91-D48A-4207-A50A-CF58A050B2B0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3470,30 +3033,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5546875" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B15</f>
         <v>03_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3501,17 +3064,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3519,112 +3082,108 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -3642,11 +3201,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{D53F624B-2FBA-41DA-94CE-9ECC22731149}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3657,30 +3212,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B19</f>
         <v>04_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3688,17 +3243,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3706,100 +3261,96 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -3817,11 +3368,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{BECBC66D-D2E1-4F15-8790-FA2BBDD000E5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3832,30 +3379,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.6640625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B23</f>
         <v>05_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3863,17 +3410,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3881,106 +3428,102 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5">
       <c r="C29" s="25"/>
     </row>
   </sheetData>
@@ -3995,11 +3538,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{707FAAF5-E9CE-4C22-B4CE-7115DE020E88}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4010,30 +3549,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B27</f>
         <v>06_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -4041,17 +3580,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -4059,108 +3598,104 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -4178,11 +3713,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{011D95A5-629E-4B01-A56E-5D0F6411D2B5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4191,31 +3722,33 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B31</f>
         <v>07_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -4223,17 +3756,17 @@
       </c>
       <c r="E3" s="43"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -4241,100 +3774,96 @@
       </c>
       <c r="E5" s="46"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="44"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -4352,11 +3881,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{E942F398-9166-4A52-A7E2-8DCF929DA045}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4364,31 +3889,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E531A025-BA5E-4614-A80F-6870F52C8D7D}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5546875" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B35</f>
         <v>08_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -4396,17 +3923,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -4414,107 +3941,103 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="15">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="47"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5" ht="14.45" customHeight="1">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="15">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B6"/>
@@ -4523,12 +4046,9 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{DDEEEEDF-A528-40A1-BB59-449213F305C7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4762,6 +4282,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
@@ -4772,49 +4301,14 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}"/>
 </file>
</xml_diff>

<commit_message>
refactor: improve audit data handling and prepare for future spinner support (#12)
- Set screenshot option to static 1 temporarily (pending Excel writer support)
- Changed run-all-lighthouse to use static data
- Updated excel-template.xlsx
- Refactored excel-writer-util:
  • Added audit option
  • Moved diagnostic and audit data gathering to dynamic functions
  • Moved screenshot adding to a dynamic function
- Refactored lighthouse-runner-util:
  • Removed some report summary logs
  • Added audits data to text-writer-util
- Refactored screenshot-util:
  • Moved diagnostic data gathering to a separate function
  • Added and moved audit data gathering to a separate function
- Added spinner-util (not yet implemented, execSync → execAsync needed)
- Refactored text-writer-util to include audits data
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29203"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cheqteams-my.sharepoint.com/personal/vwlabajo_cheqsystems_com/Documents/Documents/Team - Performance Testing/PT - Documentation/CheQ Website Production Page Speed Insight/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8EA300FF-E831-4373-BB35-1174E74F1E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{573A2E2B-B5CE-41B0-B334-BA4A05AE6729}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2009E814-DD03-4F30-B2EF-0CCF18B8CF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C37E2E45-7E9A-43D5-A28B-C770F3703849}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C37E2E45-7E9A-43D5-A28B-C770F3703849}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,24 +28,35 @@
     <definedName name="performanceRange" localSheetId="0">Summary!$L$6:$L$35</definedName>
     <definedName name="performanceValueRange" comment="This variable refers to the performance of all pages, for devices, cache, and without cache.">Summary!$L$6,Summary!$L$7,Summary!$L$10,Summary!$L$11,Summary!$L$14,Summary!$L$15,Summary!$L$18,Summary!$L$19,Summary!$L$22,Summary!$L$23,Summary!$L$26,Summary!$L$27,Summary!$L$30,Summary!$L$31</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -60,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="45">
   <si>
     <t>Lighthouse Insights</t>
   </si>
@@ -191,13 +202,7 @@
     <t>Diagnostic:</t>
   </si>
   <si>
-    <t>Defer offscreen images</t>
-  </si>
-  <si>
     <t>Recommendation:</t>
-  </si>
-  <si>
-    <t>Learn how to defer offscreen images</t>
   </si>
   <si>
     <t>Worst Insight</t>
@@ -211,7 +216,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,12 +259,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -702,7 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -812,13 +811,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -828,12 +829,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -852,9 +847,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -894,6 +886,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1081,422 +1076,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B7EB9A-6084-4497-A764-1BC71B7E8699}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2219325"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE12300-F126-4D9C-97C2-D10A8F0E5655}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2200275"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B26E2C4F-528F-4CCD-84B1-FC2BFEFFC45B}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948B4D1A-F86F-48BA-BF04-2A24804F7EAB}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EF85C6E-6393-4B76-B446-C0AB608C2980}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECEC0987-0254-40BD-8131-5086609B56A9}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2257425"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EECBFD6-95BA-4D5A-B6B9-39BC356E8EF9}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2190750"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6534150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EFADFC0-E695-49D0-B5E0-865C7C62DDBD}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF9F7BD-799B-B138-965D-EFE9317EB18A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1485900" y="2190750"/>
-          <a:ext cx="8877300" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1819,49 +1398,49 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="7" width="101.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="24.88671875" style="30" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" style="30" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="29.33203125" style="30" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" style="30" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" style="30" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5546875" style="30" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="30" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" style="30" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="29.28515625" style="30" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="30" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" style="30" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" style="30" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="56"/>
+    <row r="1" spans="1:15" ht="15" thickBot="1"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1">
+      <c r="D2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="54"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="60"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="5"/>
       <c r="J3" s="41"/>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15" thickBot="1">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1876,7 +1455,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15" thickBot="1">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="5"/>
@@ -1900,7 +1479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="26"/>
@@ -1947,8 +1526,8 @@
         <v>D7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="53" t="s">
+    <row r="7" spans="1:15" ht="15" thickBot="1">
+      <c r="B7" s="48" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1983,8 +1562,8 @@
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
     </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="54"/>
+    <row r="8" spans="1:15" ht="15" thickBot="1">
+      <c r="B8" s="49"/>
       <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
@@ -1996,7 +1575,7 @@
       <c r="N8" s="33"/>
       <c r="O8" s="33"/>
     </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15" thickBot="1">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2010,7 +1589,7 @@
       <c r="N9"/>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="26"/>
@@ -2057,8 +1636,8 @@
         <v>D11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="53" t="s">
+    <row r="11" spans="1:15" ht="15" thickBot="1">
+      <c r="B11" s="48" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -2092,8 +1671,8 @@
       <c r="N11" s="33"/>
       <c r="O11" s="33"/>
     </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="54"/>
+    <row r="12" spans="1:15" ht="15" thickBot="1">
+      <c r="B12" s="49"/>
       <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
@@ -2106,7 +1685,7 @@
       <c r="N12" s="33"/>
       <c r="O12" s="33"/>
     </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="15" thickBot="1">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="14"/>
@@ -2120,7 +1699,7 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="26"/>
@@ -2167,8 +1746,8 @@
         <v>D15</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="53" t="s">
+    <row r="15" spans="1:15" ht="15" thickBot="1">
+      <c r="B15" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -2203,8 +1782,8 @@
       <c r="N15" s="33"/>
       <c r="O15" s="33"/>
     </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="54"/>
+    <row r="16" spans="1:15" ht="15" thickBot="1">
+      <c r="B16" s="49"/>
       <c r="C16" s="10" t="s">
         <v>17</v>
       </c>
@@ -2217,7 +1796,7 @@
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
     </row>
-    <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" ht="15" thickBot="1">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="14"/>
@@ -2231,7 +1810,7 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="26"/>
@@ -2278,8 +1857,8 @@
         <v>D19</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="53" t="s">
+    <row r="19" spans="2:15" ht="15" thickBot="1">
+      <c r="B19" s="48" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -2314,8 +1893,8 @@
       <c r="N19" s="33"/>
       <c r="O19" s="33"/>
     </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="54"/>
+    <row r="20" spans="2:15" ht="15" thickBot="1">
+      <c r="B20" s="49"/>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
@@ -2328,7 +1907,7 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" ht="15" thickBot="1">
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="14"/>
@@ -2342,7 +1921,7 @@
       <c r="N21"/>
       <c r="O21"/>
     </row>
-    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="26"/>
@@ -2389,8 +1968,8 @@
         <v>D23</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="53" t="s">
+    <row r="23" spans="2:15" ht="15" thickBot="1">
+      <c r="B23" s="48" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -2425,8 +2004,8 @@
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
     </row>
-    <row r="24" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="54"/>
+    <row r="24" spans="2:15" ht="15" thickBot="1">
+      <c r="B24" s="49"/>
       <c r="C24" s="10" t="s">
         <v>17</v>
       </c>
@@ -2439,7 +2018,7 @@
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
     </row>
-    <row r="25" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:15" ht="15" thickBot="1">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="14"/>
@@ -2453,7 +2032,7 @@
       <c r="N25"/>
       <c r="O25"/>
     </row>
-    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="26"/>
@@ -2500,8 +2079,8 @@
         <v>D27</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="53" t="s">
+    <row r="27" spans="2:15" ht="15" thickBot="1">
+      <c r="B27" s="48" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -2536,8 +2115,8 @@
       <c r="N27" s="33"/>
       <c r="O27" s="33"/>
     </row>
-    <row r="28" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="54"/>
+    <row r="28" spans="2:15" ht="15" thickBot="1">
+      <c r="B28" s="49"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -2550,7 +2129,7 @@
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
     </row>
-    <row r="29" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:15" ht="15" thickBot="1">
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="14"/>
@@ -2564,7 +2143,7 @@
       <c r="N29"/>
       <c r="O29"/>
     </row>
-    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="26"/>
@@ -2611,8 +2190,8 @@
         <v>D31</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="53" t="s">
+    <row r="31" spans="2:15" ht="15" thickBot="1">
+      <c r="B31" s="48" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -2647,8 +2226,8 @@
       <c r="N31" s="33"/>
       <c r="O31" s="33"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="54"/>
+    <row r="32" spans="2:15">
+      <c r="B32" s="49"/>
       <c r="C32" s="10" t="s">
         <v>17</v>
       </c>
@@ -2661,7 +2240,7 @@
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15">
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="14"/>
@@ -2675,7 +2254,7 @@
       <c r="N33"/>
       <c r="O33"/>
     </row>
-    <row r="34" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" ht="14.45" customHeight="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="26"/>
@@ -2722,8 +2301,8 @@
         <v>D35</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="53" t="s">
+    <row r="35" spans="2:15">
+      <c r="B35" s="48" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -2758,8 +2337,8 @@
       <c r="N35" s="33"/>
       <c r="O35" s="33"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="54"/>
+    <row r="36" spans="2:15">
+      <c r="B36" s="49"/>
       <c r="C36" s="10" t="s">
         <v>17</v>
       </c>
@@ -2772,7 +2351,7 @@
       <c r="N36" s="33"/>
       <c r="O36" s="33"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:15">
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="F37" s="5"/>
@@ -2782,11 +2361,11 @@
       <c r="N37" s="33"/>
       <c r="O37" s="33"/>
     </row>
-    <row r="38" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" ht="14.45" customHeight="1">
       <c r="C38" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="47" t="s">
         <v>26</v>
       </c>
       <c r="F38" s="5"/>
@@ -2814,7 +2393,7 @@
       <c r="N38" s="33"/>
       <c r="O38" s="33"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:15">
       <c r="C39" s="12" t="s">
         <v>28</v>
       </c>
@@ -2839,7 +2418,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="33"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15">
       <c r="C40" s="13" t="s">
         <v>31</v>
       </c>
@@ -2864,7 +2443,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="33"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15">
       <c r="G41" s="51"/>
       <c r="I41" s="29" t="s">
         <v>34</v>
@@ -2882,7 +2461,7 @@
         <v>E7</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15">
       <c r="G42" s="52"/>
       <c r="I42" s="29" t="s">
         <v>35</v>
@@ -2906,7 +2485,7 @@
         <v>normal and incognito</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:15">
       <c r="I43" s="29" t="s">
         <v>36</v>
       </c>
@@ -2929,7 +2508,7 @@
       <c r="N43" s="33"/>
       <c r="O43" s="33"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:15">
       <c r="I44" s="29" t="s">
         <v>37</v>
       </c>
@@ -2960,7 +2539,7 @@
         <v>B6</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15">
       <c r="I45" s="29" t="s">
         <v>38</v>
       </c>
@@ -2973,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15">
       <c r="I46" s="29" t="s">
         <v>39</v>
       </c>
@@ -2986,7 +2565,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15">
       <c r="J47" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J47" ca="1">INDIRECT(J48)</f>
         <v>01_url</v>
@@ -2996,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15">
       <c r="J48" s="30" t="str" cm="1">
         <f t="array" aca="1" ref="J48" ca="1">LEFT(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0)-1)&amp;(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44))-(MOD(MID(J44,MATCH(TRUE,ISNUMBER(MID(J44,ROW(INDIRECT("1:"&amp;LEN(J44))),1)+0),0),LEN(J44)),2)=0))</f>
         <v>B7</v>
@@ -3008,15 +2587,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="G10:G12"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="G38:G42"/>
     <mergeCell ref="B19:B20"/>
@@ -3028,68 +2598,77 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="G34:G36"/>
     <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="G10:G12"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:E8">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="D35:E36">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:E32">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:E28">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:E24">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:E20">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
+      <formula>90</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:E16">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:E12">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:E16">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="D7:E8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19:E20">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23:E24">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:E28">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31:E32">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="14" operator="lessThan">
-      <formula>90</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:E36">
-    <cfRule type="cellIs" dxfId="1" priority="15" operator="lessThan">
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>90</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3104,30 +2683,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.109375" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B7</f>
         <v>01_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3135,17 +2714,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3153,106 +2732,102 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="29" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:5" ht="14.45" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C26:E26"/>
@@ -3265,11 +2840,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{958DC036-E7D9-4E9F-92F1-E9C4EDA77823}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3280,30 +2851,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.109375" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B11</f>
         <v>02_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3311,17 +2882,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3329,118 +2900,114 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5">
       <c r="C30" s="25"/>
     </row>
   </sheetData>
@@ -3455,11 +3022,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{9D988C91-D48A-4207-A50A-CF58A050B2B0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3470,30 +3033,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5546875" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B15</f>
         <v>03_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3501,17 +3064,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3519,112 +3082,108 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -3642,11 +3201,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{D53F624B-2FBA-41DA-94CE-9ECC22731149}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3657,30 +3212,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B19</f>
         <v>04_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3688,17 +3243,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3706,100 +3261,96 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -3817,11 +3368,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{BECBC66D-D2E1-4F15-8790-FA2BBDD000E5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3832,30 +3379,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.6640625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B23</f>
         <v>05_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -3863,17 +3410,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -3881,106 +3428,102 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5">
       <c r="C29" s="25"/>
     </row>
   </sheetData>
@@ -3995,11 +3538,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{707FAAF5-E9CE-4C22-B4CE-7115DE020E88}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4010,30 +3549,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="64">
+    <row r="1" spans="2:5" ht="15" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1">
+      <c r="C2" s="59">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1">
+      <c r="B3" s="61" t="str">
         <f>Summary!B27</f>
         <v>06_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -4041,17 +3580,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5" ht="15" thickBot="1">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -4059,108 +3598,104 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5" ht="15" thickBot="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="15" thickBot="1">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -4178,11 +3713,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{011D95A5-629E-4B01-A56E-5D0F6411D2B5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4191,31 +3722,33 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B31</f>
         <v>07_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -4223,17 +3756,17 @@
       </c>
       <c r="E3" s="43"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -4241,100 +3774,96 @@
       </c>
       <c r="E5" s="46"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="44"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="76"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15" thickBot="1">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5" ht="15" thickBot="1">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5" ht="15" thickBot="1">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
@@ -4352,11 +3881,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{E942F398-9166-4A52-A7E2-8DCF929DA045}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4364,31 +3889,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E531A025-BA5E-4614-A80F-6870F52C8D7D}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5546875" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-    <col min="7" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5703125" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="64">
+    <row r="2" spans="2:5">
+      <c r="C2" s="59">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="66" t="str">
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="61" t="str">
         <f>Summary!B35</f>
         <v>08_url</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -4396,17 +3923,17 @@
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
-      <c r="C4" s="70"/>
+    <row r="4" spans="2:5">
+      <c r="B4" s="62"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="67"/>
-      <c r="C5" s="70" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="62"/>
+      <c r="C5" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -4414,107 +3941,103 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="71"/>
+    <row r="6" spans="2:5">
+      <c r="B6" s="63"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="15">
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="67">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-    </row>
-    <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="2:5" ht="14.45" customHeight="1">
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+    </row>
+    <row r="11" spans="2:5" ht="14.45" customHeight="1">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="47"/>
-    </row>
-    <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="78"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+    </row>
+    <row r="12" spans="2:5" ht="14.45" customHeight="1">
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="15">
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5">
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5">
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5">
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="67">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="74"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B6"/>
@@ -4523,12 +4046,9 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://developer.chrome.com/docs/lighthouse/performance/offscreen-images/?utm_source=lighthouse&amp;utm_medium=lr" xr:uid="{DDEEEEDF-A528-40A1-BB59-449213F305C7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4762,6 +4282,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
@@ -4772,49 +4301,14 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}"/>
 </file>
</xml_diff>

<commit_message>
refactor(core, config, template): major async update and cleanup (#14)
- Change naming in lighthouse.config.ts: `excelOutputName` → `excelTemplateFileName`
- Refactor run-all-lighthouse.ts: relocate file arrangement logic from lighthouse-runner-util.ts
- Update excel-template structure for improved organization
- Remove unnecessary console log for successful screenshots
- Major refactor: replace execSync with spawn for async handling
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VonWebsterDLabajo\VS Code\Lighthouse-Playwright-Typescript-Automation\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C742699-5E0F-4367-86A1-60DCF1AF992F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C869E7D0-6CCD-40B6-AE49-87CECD4F9A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F6E278F-D365-4345-BA7B-50EDF112F8F8}"/>
   </bookViews>
@@ -727,7 +727,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -839,6 +839,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -857,20 +872,26 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -895,33 +916,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1523,22 +1517,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="48"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="52"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1571,7 +1565,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="55" t="str">
+      <c r="G6" s="47" t="str">
         <f>IF(OR(ISBLANK(D6),ISBLANK(E6),TEXT(D6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D6,TEXT(E6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E6),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L6=0,Formula_Sheet!L7=0),
@@ -1584,7 +1578,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="50" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1593,17 +1587,17 @@
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="56"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="54"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="57"/>
+      <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
@@ -1619,7 +1613,7 @@
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="55" t="str">
+      <c r="G10" s="47" t="str">
         <f>IF(OR(ISBLANK(D10),ISBLANK(E10),TEXT(D10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D10,TEXT(E10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E10),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L10=0,Formula_Sheet!L11=0),
@@ -1632,7 +1626,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="50" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1640,17 +1634,17 @@
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
-      <c r="G11" s="56"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="54"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="57"/>
+      <c r="G12" s="49"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
@@ -1666,7 +1660,7 @@
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="55" t="str">
+      <c r="G14" s="47" t="str">
         <f>IF(OR(ISBLANK(D14),ISBLANK(E14),TEXT(D14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D14,TEXT(E14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E14),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L14=0,Formula_Sheet!L15=0),
@@ -1679,7 +1673,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="50" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1688,17 +1682,17 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="56"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="54"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="57"/>
+      <c r="G16" s="49"/>
     </row>
     <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
@@ -1714,7 +1708,7 @@
       <c r="D18" s="42"/>
       <c r="E18" s="23"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="55" t="str">
+      <c r="G18" s="47" t="str">
         <f>IF(OR(ISBLANK(D18),ISBLANK(E18),TEXT(D18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D18,TEXT(E18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E18),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L18=0,Formula_Sheet!L19=0),
@@ -1727,7 +1721,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="50" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1736,17 +1730,17 @@
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="56"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="54"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="57"/>
+      <c r="G20" s="49"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
@@ -1762,7 +1756,7 @@
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="55" t="str">
+      <c r="G22" s="47" t="str">
         <f>IF(OR(ISBLANK(D22),ISBLANK(E22),TEXT(D22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D22,TEXT(E22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E22),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L22=0,Formula_Sheet!L23=0),
@@ -1775,7 +1769,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="50" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -1784,17 +1778,17 @@
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="56"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="54"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="57"/>
+      <c r="G24" s="49"/>
     </row>
     <row r="25" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
@@ -1810,7 +1804,7 @@
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="55" t="str">
+      <c r="G26" s="47" t="str">
         <f>IF(OR(ISBLANK(D26),ISBLANK(E26),TEXT(D26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D26,TEXT(E26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E26),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L26=0,Formula_Sheet!L27=0),
@@ -1823,7 +1817,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="50" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -1832,17 +1826,17 @@
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="56"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="54"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="57"/>
+      <c r="G28" s="49"/>
     </row>
     <row r="29" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
@@ -1858,7 +1852,7 @@
       <c r="D30" s="23"/>
       <c r="E30" s="42"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="55" t="str">
+      <c r="G30" s="47" t="str">
         <f>IF(OR(ISBLANK(D30),ISBLANK(E30),TEXT(D30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D30,TEXT(E30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E30),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L30=0,Formula_Sheet!L31=0),
@@ -1871,7 +1865,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="50" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -1880,17 +1874,17 @@
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="56"/>
+      <c r="G31" s="48"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="54"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="57"/>
+      <c r="G32" s="49"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
@@ -1906,7 +1900,7 @@
       <c r="D34" s="23"/>
       <c r="E34" s="42"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="55" t="str">
+      <c r="G34" s="47" t="str">
         <f>IF(OR(ISBLANK(D34),ISBLANK(E34),TEXT(D34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D34,TEXT(E34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E34),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L34=0,Formula_Sheet!L35=0),
@@ -1919,7 +1913,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="50" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -1928,17 +1922,17 @@
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="56"/>
+      <c r="G35" s="48"/>
     </row>
     <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="54"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="57"/>
+      <c r="G36" s="49"/>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
@@ -1954,7 +1948,7 @@
         <v>16</v>
       </c>
       <c r="F38" s="6"/>
-      <c r="G38" s="55" t="str" cm="1">
+      <c r="G38" s="47" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">IF(OR(Formula_Sheet!J39=0,Formula_Sheet!K39=0),
 "Kindly, fill the Performance Score first!",
 "The best recorded performance score was in the " &amp; Formula_Sheet!J46 &amp; " page for " &amp; INDIRECT(Formula_Sheet!J43) &amp; " devices " &amp; Formula_Sheet!J35 &amp; ", at " &amp; Formula_Sheet!J39 &amp; CHAR(10) &amp;
@@ -1973,7 +1967,7 @@
         <v>19</v>
       </c>
       <c r="F39" s="6"/>
-      <c r="G39" s="56"/>
+      <c r="G39" s="48"/>
     </row>
     <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="13" t="s">
@@ -1983,16 +1977,21 @@
         <v>22</v>
       </c>
       <c r="F40" s="6"/>
-      <c r="G40" s="56"/>
+      <c r="G40" s="48"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G41" s="56"/>
+      <c r="G41" s="48"/>
     </row>
     <row r="42" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G42" s="57"/>
+      <c r="G42" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="G38:G42"/>
@@ -2008,11 +2007,6 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="G14:G16"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E8">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
@@ -2928,18 +2922,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B7</f>
         <v>01_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -2948,16 +2942,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2966,8 +2960,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -2987,28 +2981,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3039,41 +3031,41 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3098,18 +3090,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B11</f>
         <v>02_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3118,16 +3110,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3136,8 +3128,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3157,28 +3149,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3200,6 +3190,18 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
     <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>34</v>
@@ -3209,28 +3211,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C30" s="22"/>
@@ -3271,18 +3273,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B15</f>
         <v>03_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3291,16 +3293,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3309,8 +3311,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3330,28 +3332,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3382,28 +3382,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3441,18 +3441,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B19</f>
         <v>04_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3461,16 +3461,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3479,8 +3479,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3500,28 +3500,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3543,6 +3541,18 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
     <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>34</v>
@@ -3552,28 +3562,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3611,18 +3621,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B23</f>
         <v>05_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3631,16 +3641,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3649,8 +3659,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3670,28 +3680,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3713,6 +3721,18 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
     <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>34</v>
@@ -3722,28 +3742,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C29" s="22"/>
@@ -3784,18 +3804,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B27</f>
         <v>06_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3804,16 +3824,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3822,8 +3842,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3843,28 +3863,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3886,6 +3904,18 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
     <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>34</v>
@@ -3895,28 +3925,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3953,18 +3983,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B31</f>
         <v>07_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3973,16 +4003,16 @@
       <c r="E3" s="38"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="40"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3991,8 +4021,8 @@
       <c r="E5" s="41"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -4012,28 +4042,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -4064,28 +4092,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4122,18 +4150,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="58">
+      <c r="C2" s="69">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="71" t="str">
         <f>Summary!B35</f>
         <v>08_Link</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="74" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -4142,16 +4170,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="61"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -4160,8 +4188,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="62"/>
-      <c r="C6" s="65"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -4172,37 +4200,35 @@
       <c r="C7" s="15"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="62">
         <f>E3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -4224,37 +4250,49 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="62">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4274,26 +4312,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D539BB261075264EADE6FB64A6A44314" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8545620b90e3ca3b4fa9c0eed4ef96d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851fd863-1f96-44b1-878a-247793b557e9" xmlns:ns3="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2cedb268f8f7bfc874339ceeb7c9957" ns2:_="" ns3:_="">
     <xsd:import namespace="851fd863-1f96-44b1-878a-247793b557e9"/>
@@ -4522,10 +4540,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4548,20 +4597,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor(reporting): improve report sharing and structure
- Refactor run-all-lighthouse.ts timestamp handling
- Update Excel template
- Refactor excel-writer-util: use formula HYPERLINK instead of direct hyperlink for better sharability
- Remove unnecessary import
- Refactor report-path-util.ts: add timestamp in HTML folder path for easier file sharing
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VonWebsterDLabajo\VS Code\Lighthouse-Playwright-Typescript-Automation\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C869E7D0-6CCD-40B6-AE49-87CECD4F9A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87151153-D487-481F-AFC9-562854B0A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F6E278F-D365-4345-BA7B-50EDF112F8F8}"/>
   </bookViews>
@@ -184,9 +184,6 @@
     <t>Analysis Results</t>
   </si>
   <si>
-    <t>Lighthouse Insights</t>
-  </si>
-  <si>
     <t>Websites</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>08_Link</t>
+  </si>
+  <si>
+    <t>Lighthouse Report</t>
   </si>
 </sst>
 </file>
@@ -839,6 +839,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -848,74 +872,50 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1517,22 +1517,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="53"/>
+      <c r="D2" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="48"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
-      <c r="B3" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56" t="s">
+      <c r="B3" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="57"/>
+      <c r="E3" s="52"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1565,7 +1565,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="47" t="str">
+      <c r="G6" s="55" t="str">
         <f>IF(OR(ISBLANK(D6),ISBLANK(E6),TEXT(D6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D6,TEXT(E6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E6),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L6=0,Formula_Sheet!L7=0),
@@ -1578,8 +1578,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="50" t="s">
-        <v>38</v>
+      <c r="B7" s="53" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
@@ -1587,17 +1587,17 @@
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="48"/>
+      <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="51"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="49"/>
+      <c r="G8" s="57"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
@@ -1613,7 +1613,7 @@
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="47" t="str">
+      <c r="G10" s="55" t="str">
         <f>IF(OR(ISBLANK(D10),ISBLANK(E10),TEXT(D10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D10,TEXT(E10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E10),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L10=0,Formula_Sheet!L11=0),
@@ -1626,25 +1626,25 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="50" t="s">
-        <v>39</v>
+      <c r="B11" s="53" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
-      <c r="G11" s="48"/>
+      <c r="G11" s="56"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="51"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="49"/>
+      <c r="G12" s="57"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
@@ -1660,7 +1660,7 @@
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="47" t="str">
+      <c r="G14" s="55" t="str">
         <f>IF(OR(ISBLANK(D14),ISBLANK(E14),TEXT(D14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D14,TEXT(E14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E14),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L14=0,Formula_Sheet!L15=0),
@@ -1673,8 +1673,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="50" t="s">
-        <v>40</v>
+      <c r="B15" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>12</v>
@@ -1682,17 +1682,17 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="48"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="51"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="49"/>
+      <c r="G16" s="57"/>
     </row>
     <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
@@ -1708,7 +1708,7 @@
       <c r="D18" s="42"/>
       <c r="E18" s="23"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="47" t="str">
+      <c r="G18" s="55" t="str">
         <f>IF(OR(ISBLANK(D18),ISBLANK(E18),TEXT(D18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D18,TEXT(E18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E18),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L18=0,Formula_Sheet!L19=0),
@@ -1721,8 +1721,8 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="50" t="s">
-        <v>41</v>
+      <c r="B19" s="53" t="s">
+        <v>40</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>12</v>
@@ -1730,17 +1730,17 @@
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="48"/>
+      <c r="G19" s="56"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="51"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="49"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
@@ -1756,7 +1756,7 @@
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="47" t="str">
+      <c r="G22" s="55" t="str">
         <f>IF(OR(ISBLANK(D22),ISBLANK(E22),TEXT(D22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D22,TEXT(E22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E22),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L22=0,Formula_Sheet!L23=0),
@@ -1769,8 +1769,8 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="50" t="s">
-        <v>42</v>
+      <c r="B23" s="53" t="s">
+        <v>41</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>12</v>
@@ -1778,17 +1778,17 @@
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="48"/>
+      <c r="G23" s="56"/>
     </row>
     <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="51"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="49"/>
+      <c r="G24" s="57"/>
     </row>
     <row r="25" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
@@ -1804,7 +1804,7 @@
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="47" t="str">
+      <c r="G26" s="55" t="str">
         <f>IF(OR(ISBLANK(D26),ISBLANK(E26),TEXT(D26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D26,TEXT(E26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E26),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L26=0,Formula_Sheet!L27=0),
@@ -1817,8 +1817,8 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="50" t="s">
-        <v>43</v>
+      <c r="B27" s="53" t="s">
+        <v>42</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>12</v>
@@ -1826,17 +1826,17 @@
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="48"/>
+      <c r="G27" s="56"/>
     </row>
     <row r="28" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="51"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="49"/>
+      <c r="G28" s="57"/>
     </row>
     <row r="29" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
@@ -1852,7 +1852,7 @@
       <c r="D30" s="23"/>
       <c r="E30" s="42"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="47" t="str">
+      <c r="G30" s="55" t="str">
         <f>IF(OR(ISBLANK(D30),ISBLANK(E30),TEXT(D30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D30,TEXT(E30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E30),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L30=0,Formula_Sheet!L31=0),
@@ -1865,8 +1865,8 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="50" t="s">
-        <v>44</v>
+      <c r="B31" s="53" t="s">
+        <v>43</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>12</v>
@@ -1874,17 +1874,17 @@
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="48"/>
+      <c r="G31" s="56"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="51"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="49"/>
+      <c r="G32" s="57"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
@@ -1900,7 +1900,7 @@
       <c r="D34" s="23"/>
       <c r="E34" s="42"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="47" t="str">
+      <c r="G34" s="55" t="str">
         <f>IF(OR(ISBLANK(D34),ISBLANK(E34),TEXT(D34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D34,TEXT(E34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E34),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!L34=0,Formula_Sheet!L35=0),
@@ -1913,8 +1913,8 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="50" t="s">
-        <v>45</v>
+      <c r="B35" s="53" t="s">
+        <v>44</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>12</v>
@@ -1922,17 +1922,17 @@
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="48"/>
+      <c r="G35" s="56"/>
     </row>
     <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="51"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="49"/>
+      <c r="G36" s="57"/>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
@@ -1948,7 +1948,7 @@
         <v>16</v>
       </c>
       <c r="F38" s="6"/>
-      <c r="G38" s="47" t="str" cm="1">
+      <c r="G38" s="55" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1">IF(OR(Formula_Sheet!J39=0,Formula_Sheet!K39=0),
 "Kindly, fill the Performance Score first!",
 "The best recorded performance score was in the " &amp; Formula_Sheet!J46 &amp; " page for " &amp; INDIRECT(Formula_Sheet!J43) &amp; " devices " &amp; Formula_Sheet!J35 &amp; ", at " &amp; Formula_Sheet!J39 &amp; CHAR(10) &amp;
@@ -1967,7 +1967,7 @@
         <v>19</v>
       </c>
       <c r="F39" s="6"/>
-      <c r="G39" s="48"/>
+      <c r="G39" s="56"/>
     </row>
     <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="13" t="s">
@@ -1977,21 +1977,16 @@
         <v>22</v>
       </c>
       <c r="F40" s="6"/>
-      <c r="G40" s="48"/>
+      <c r="G40" s="56"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G41" s="48"/>
+      <c r="G41" s="56"/>
     </row>
     <row r="42" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G42" s="49"/>
+      <c r="G42" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="G38:G42"/>
@@ -2007,6 +2002,11 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="G14:G16"/>
     <mergeCell ref="G10:G12"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E8">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
@@ -2922,18 +2922,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B7</f>
         <v>01_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -2942,16 +2942,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2960,8 +2960,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -2981,26 +2981,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3031,41 +3031,41 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3090,18 +3090,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B11</f>
         <v>02_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3110,16 +3110,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3128,8 +3128,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3149,26 +3149,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3211,28 +3211,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C30" s="22"/>
@@ -3273,18 +3273,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B15</f>
         <v>03_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3293,16 +3293,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3311,8 +3311,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3332,26 +3332,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3382,28 +3382,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3441,18 +3441,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B19</f>
         <v>04_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3461,16 +3461,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3479,8 +3479,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3500,26 +3500,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3562,28 +3562,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3621,18 +3621,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B23</f>
         <v>05_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3641,16 +3641,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3659,8 +3659,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3680,26 +3680,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3742,28 +3742,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C29" s="22"/>
@@ -3804,18 +3804,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B27</f>
         <v>06_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -3824,16 +3824,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3842,8 +3842,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -3863,26 +3863,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -3925,28 +3925,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3983,18 +3983,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B31</f>
         <v>07_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -4003,16 +4003,16 @@
       <c r="E3" s="38"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="40"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -4021,8 +4021,8 @@
       <c r="E5" s="41"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -4042,26 +4042,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -4092,28 +4092,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4150,18 +4150,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="69">
+      <c r="C2" s="58">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="60" t="str">
         <f>Summary!B35</f>
         <v>08_Link</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -4170,16 +4170,16 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="72"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -4188,8 +4188,8 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="76"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
@@ -4209,26 +4209,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="62">
-        <f>E3</f>
+      <c r="C9" s="66">
+        <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="17"/>
@@ -4271,28 +4271,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="66">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="61"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4312,6 +4312,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D539BB261075264EADE6FB64A6A44314" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8545620b90e3ca3b4fa9c0eed4ef96d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851fd863-1f96-44b1-878a-247793b557e9" xmlns:ns3="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2cedb268f8f7bfc874339ceeb7c9957" ns2:_="" ns3:_="">
     <xsd:import namespace="851fd863-1f96-44b1-878a-247793b557e9"/>
@@ -4540,41 +4560,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4597,9 +4586,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor(excel): move module location and update complex formula to array in Formula_Sheet
- updated complex formula as array in Formula_Sheet to prevent errors when copying
- refactored module location for better structure
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VonWebsterDLabajo\VS Code\Lighthouse-Playwright-Typescript-Automation\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F989AF-5DF9-4059-81CB-3096A2CA774B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA507479-F7D3-4D19-BB2E-1E68D51105C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3D68101-3EA1-4AB8-9C35-12A619CAE77F}"/>
   </bookViews>
@@ -1149,6 +1149,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1158,29 +1182,38 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1194,44 +1227,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1829,22 +1829,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="72"/>
+      <c r="E2" s="67"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="76"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="71"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1877,7 +1877,7 @@
       <c r="D6" s="61"/>
       <c r="E6" s="61"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="66" t="str">
+      <c r="G6" s="74" t="str">
         <f>IF(OR(ISBLANK(D6),ISBLANK(E6),TEXT(D6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D6,TEXT(E6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E6),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K6=0,Formula_Sheet!N6=0),
@@ -1890,7 +1890,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="72" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1899,17 +1899,17 @@
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="67"/>
+      <c r="G7" s="75"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="70"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="68"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
@@ -1925,7 +1925,7 @@
       <c r="D10" s="61"/>
       <c r="E10" s="61"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="66" t="str">
+      <c r="G10" s="74" t="str">
         <f>IF(OR(ISBLANK(D10),ISBLANK(E10),TEXT(D10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D10,TEXT(E10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E10),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K10=0,Formula_Sheet!N10=0),
@@ -1938,7 +1938,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="72" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1946,17 +1946,17 @@
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
-      <c r="G11" s="67"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="70"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="68"/>
+      <c r="G12" s="76"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
@@ -1972,7 +1972,7 @@
       <c r="D14" s="61"/>
       <c r="E14" s="61"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="66" t="str">
+      <c r="G14" s="74" t="str">
         <f>IF(OR(ISBLANK(D14),ISBLANK(E14),TEXT(D14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D14,TEXT(E14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E14),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K14=0,Formula_Sheet!N14=0),
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="72" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1994,17 +1994,17 @@
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="67"/>
+      <c r="G15" s="75"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="70"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="68"/>
+      <c r="G16" s="76"/>
     </row>
     <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
@@ -2020,7 +2020,7 @@
       <c r="D18" s="63"/>
       <c r="E18" s="61"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="66" t="str">
+      <c r="G18" s="74" t="str">
         <f>IF(OR(ISBLANK(D18),ISBLANK(E18),TEXT(D18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D18,TEXT(E18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E18),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K18=0,Formula_Sheet!N18=0),
@@ -2033,7 +2033,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="72" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -2042,17 +2042,17 @@
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="67"/>
+      <c r="G19" s="75"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="70"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="68"/>
+      <c r="G20" s="76"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
@@ -2068,7 +2068,7 @@
       <c r="D22" s="61"/>
       <c r="E22" s="61"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="66" t="str">
+      <c r="G22" s="74" t="str">
         <f>IF(OR(ISBLANK(D22),ISBLANK(E22),TEXT(D22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D22,TEXT(E22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E22),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K22=0,Formula_Sheet!N22=0),
@@ -2081,7 +2081,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="72" t="s">
         <v>87</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -2090,17 +2090,17 @@
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="67"/>
+      <c r="G23" s="75"/>
     </row>
     <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="70"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="68"/>
+      <c r="G24" s="76"/>
     </row>
     <row r="25" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
@@ -2116,7 +2116,7 @@
       <c r="D26" s="61"/>
       <c r="E26" s="61"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="66" t="str">
+      <c r="G26" s="74" t="str">
         <f>IF(OR(ISBLANK(D26),ISBLANK(E26),TEXT(D26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D26,TEXT(E26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E26),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K26=0,Formula_Sheet!N26=0),
@@ -2129,7 +2129,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="72" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -2138,17 +2138,17 @@
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="67"/>
+      <c r="G27" s="75"/>
     </row>
     <row r="28" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="70"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="68"/>
+      <c r="G28" s="76"/>
     </row>
     <row r="29" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
@@ -2164,7 +2164,7 @@
       <c r="D30" s="61"/>
       <c r="E30" s="63"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="66" t="str">
+      <c r="G30" s="74" t="str">
         <f>IF(OR(ISBLANK(D30),ISBLANK(E30),TEXT(D30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D30,TEXT(E30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E30),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K30=0,Formula_Sheet!N30=0),
@@ -2177,7 +2177,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="72" t="s">
         <v>89</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -2186,17 +2186,17 @@
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="67"/>
+      <c r="G31" s="75"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="70"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="68"/>
+      <c r="G32" s="76"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
@@ -2212,7 +2212,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="63"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="66" t="str">
+      <c r="G34" s="74" t="str">
         <f>IF(OR(ISBLANK(D34),ISBLANK(E34),TEXT(D34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D34,TEXT(E34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E34),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K34=0,Formula_Sheet!N34=0),
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="69" t="s">
+      <c r="B35" s="72" t="s">
         <v>90</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -2234,17 +2234,17 @@
       <c r="D35" s="43"/>
       <c r="E35" s="43"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="67"/>
+      <c r="G35" s="75"/>
     </row>
     <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="70"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="68"/>
+      <c r="G36" s="76"/>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
@@ -2260,7 +2260,7 @@
         <v>16</v>
       </c>
       <c r="F38" s="6"/>
-      <c r="G38" s="66" t="str">
+      <c r="G38" s="74" t="str">
         <f>IF(OR(Formula_Sheet!J39=0,Formula_Sheet!K39=0),
 "Kindly, fill the Performance Score first!",
 Formula_Sheet!T61 &amp; Formula_Sheet!T62 &amp;
@@ -2282,7 +2282,7 @@
         <v>19</v>
       </c>
       <c r="F39" s="6"/>
-      <c r="G39" s="67"/>
+      <c r="G39" s="75"/>
     </row>
     <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="13" t="s">
@@ -2292,21 +2292,16 @@
         <v>22</v>
       </c>
       <c r="F40" s="6"/>
-      <c r="G40" s="67"/>
+      <c r="G40" s="75"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G41" s="67"/>
+      <c r="G41" s="75"/>
     </row>
     <row r="42" spans="2:7" ht="64.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G42" s="68"/>
+      <c r="G42" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="G38:G42"/>
@@ -2322,6 +2317,11 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="G14:G16"/>
     <mergeCell ref="G10:G12"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E8">
     <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
@@ -2421,8 +2421,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="I3:AP64"/>
   <sheetViews>
-    <sheetView topLeftCell="W43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF50" sqref="AF50"/>
+    <sheetView topLeftCell="S27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V50" sqref="V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5101,40 +5101,40 @@
       <c r="U39" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="V39" s="23" cm="1">
-        <f t="array" aca="1" ref="V39:V46" ca="1">_xlfn._xlws.FILTER(T39:T46, T39:T46=MAX(T39:T46))</f>
-        <v>0</v>
-      </c>
-      <c r="W39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="W39:W46" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(T39:T46), COLUMN(T39:T46), 4), T39:T46=MAX(T39:T46))</f>
+      <c r="V39" s="23">
+        <f t="array" aca="1" ref="V39" ca="1">_xlfn._xlws.FILTER(T39:T46, T39:T46=MAX(T39:T46))</f>
+        <v>0</v>
+      </c>
+      <c r="W39" s="23" t="str">
+        <f t="array" aca="1" ref="W39" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(T39:T46), COLUMN(T39:T46), 4), T39:T46=MAX(T39:T46))</f>
         <v>T39</v>
       </c>
-      <c r="X39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="X39:X46" ca="1">_xlfn._xlws.FILTER(U39:U46, T39:T46=MAX(T39:T46))</f>
+      <c r="X39" s="23" t="str">
+        <f t="array" aca="1" ref="X39" ca="1">_xlfn._xlws.FILTER(U39:U46, T39:T46=MAX(T39:T46))</f>
         <v>K6</v>
       </c>
-      <c r="Y39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="Y39:Y46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2))))</f>
+      <c r="Y39" s="23" t="str">
+        <f t="array" aca="1" ref="Y39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2))))</f>
         <v>01_First Link</v>
       </c>
       <c r="Z39" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y39))</f>
-        <v>01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 06_Sixth Link, 07_Seventh Link, 08_Eighth Link</v>
-      </c>
-      <c r="AA39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="AA39:AA46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)))+1, 999)))</f>
+        <f t="array" aca="1" ref="Z39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y39))</f>
+        <v>01_First Link</v>
+      </c>
+      <c r="AA39" s="23" t="str">
+        <f t="array" aca="1" ref="AA39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)))+1, 999)))</f>
         <v>First Link</v>
       </c>
       <c r="AB39" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA39))</f>
-        <v>First Link, Second Link, Third Link, Fourth Link, Fifth Link, Sixth Link, Seventh Link, Eighth Link</v>
-      </c>
-      <c r="AC39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="AC39:AC46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+        <f t="array" aca="1" ref="AB39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA39))</f>
+        <v>First Link</v>
+      </c>
+      <c r="AC39" s="23" t="str">
+        <f t="array" aca="1" ref="AC39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AD39" s="46" t="str" cm="1">
-        <f t="array" aca="1" ref="AD39:AD46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+      <c r="AD39" s="46" t="str">
+        <f t="array" aca="1" ref="AD39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
       <c r="AF39" s="54">
@@ -5144,40 +5144,40 @@
       <c r="AG39" t="s">
         <v>61</v>
       </c>
-      <c r="AH39" cm="1">
-        <f t="array" aca="1" ref="AH39:AH45" ca="1">_xlfn._xlws.FILTER(AF39:AF46, AF39:AF46=MIN(AF39:AF46))</f>
-        <v>0</v>
-      </c>
-      <c r="AI39" t="str" cm="1">
-        <f t="array" aca="1" ref="AI39:AI45" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(AF39:AF46), COLUMN(AF39:AF46), 4), AF39:AF46=MIN(AF39:AF46))</f>
+      <c r="AH39">
+        <f t="array" aca="1" ref="AH39" ca="1">_xlfn._xlws.FILTER(AF39:AF46, AF39:AF46=MIN(AF39:AF46))</f>
+        <v>0</v>
+      </c>
+      <c r="AI39" t="str">
+        <f t="array" aca="1" ref="AI39" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(AF39:AF46), COLUMN(AF39:AF46), 4), AF39:AF46=MIN(AF39:AF46))</f>
         <v>AF39</v>
       </c>
-      <c r="AJ39" t="str" cm="1">
-        <f t="array" aca="1" ref="AJ39:AJ45" ca="1">_xlfn._xlws.FILTER(AG39:AG46, AF39:AF46=MIN(AF39:AF46))</f>
+      <c r="AJ39" t="str">
+        <f t="array" aca="1" ref="AJ39" ca="1">_xlfn._xlws.FILTER(AG39:AG46, AF39:AF46=MIN(AF39:AF46))</f>
         <v>N6</v>
       </c>
-      <c r="AK39" t="str" cm="1">
-        <f t="array" aca="1" ref="AK39:AK45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5))))</f>
+      <c r="AK39" t="str">
+        <f t="array" aca="1" ref="AK39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5))))</f>
         <v>01_First Link</v>
       </c>
       <c r="AL39" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE, AK39, AK40, AK41, AK42, AK43, AK44, AK45, AK46)</f>
-        <v>01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 07_Seventh Link, 08_Eighth Link</v>
-      </c>
-      <c r="AM39" t="str" cm="1">
-        <f t="array" aca="1" ref="AM39:AM45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)))+1, 999)))</f>
+        <f t="array" aca="1" ref="AL39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AK39))</f>
+        <v>01_First Link</v>
+      </c>
+      <c r="AM39" t="str">
+        <f t="array" aca="1" ref="AM39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39),_xlfn.LAMBDA(_xlpm.cell_address,MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1,COLUMN(INDIRECT(_xlpm.cell_address))-5)),FIND("_",INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1,COLUMN(INDIRECT(_xlpm.cell_address))-5)))+1,999)))</f>
         <v>First Link</v>
       </c>
       <c r="AN39" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE, AM39, AM40, AM41, AM42, AM43, AM44, AM45, AM46)</f>
-        <v>First Link, Second Link, Third Link, Fourth Link, Fifth Link, Seventh Link, Eighth Link</v>
-      </c>
-      <c r="AO39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="AO39:AO45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+        <f t="array" aca="1" ref="AN39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AM39))</f>
+        <v>First Link</v>
+      </c>
+      <c r="AO39" s="23" t="str">
+        <f t="array" aca="1" ref="AO39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AP39" s="46" t="str" cm="1">
-        <f t="array" aca="1" ref="AP39:AP45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+      <c r="AP39" s="46" t="str">
+        <f t="array" aca="1" ref="AP39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
     </row>
@@ -5204,36 +5204,15 @@
       <c r="U40" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="V40" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W40" s="23" t="str">
-        <f ca="1"/>
-        <v>T40</v>
-      </c>
-      <c r="X40" s="23" t="str">
-        <f ca="1"/>
-        <v>K10</v>
-      </c>
-      <c r="Y40" s="23" t="str">
-        <f ca="1"/>
-        <v>02_Second Link</v>
-      </c>
+      <c r="V40" s="23"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
       <c r="Z40" s="23"/>
-      <c r="AA40" s="23" t="str">
-        <f ca="1"/>
-        <v>Second Link</v>
-      </c>
+      <c r="AA40" s="23"/>
       <c r="AB40" s="23"/>
-      <c r="AC40" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD40" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC40" s="23"/>
+      <c r="AD40" s="46"/>
       <c r="AF40" s="54">
         <f ca="1">IF(M11="with and without cache", N10, FALSE)</f>
         <v>0</v>
@@ -5241,34 +5220,7 @@
       <c r="AG40" t="s">
         <v>62</v>
       </c>
-      <c r="AH40">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI40" t="str">
-        <f ca="1"/>
-        <v>AF40</v>
-      </c>
-      <c r="AJ40" t="str">
-        <f ca="1"/>
-        <v>N10</v>
-      </c>
-      <c r="AK40" t="str">
-        <f ca="1"/>
-        <v>02_Second Link</v>
-      </c>
-      <c r="AM40" t="str">
-        <f ca="1"/>
-        <v>Second Link</v>
-      </c>
-      <c r="AO40" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP40" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP40" s="53"/>
     </row>
     <row r="41" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I41" s="22" t="s">
@@ -5293,36 +5245,15 @@
       <c r="U41" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="V41" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W41" s="23" t="str">
-        <f ca="1"/>
-        <v>T41</v>
-      </c>
-      <c r="X41" s="23" t="str">
-        <f ca="1"/>
-        <v>K14</v>
-      </c>
-      <c r="Y41" s="23" t="str">
-        <f ca="1"/>
-        <v>03_Third Link</v>
-      </c>
+      <c r="V41" s="23"/>
+      <c r="W41" s="23"/>
+      <c r="X41" s="23"/>
+      <c r="Y41" s="23"/>
       <c r="Z41" s="23"/>
-      <c r="AA41" s="23" t="str">
-        <f ca="1"/>
-        <v>Third Link</v>
-      </c>
+      <c r="AA41" s="23"/>
       <c r="AB41" s="23"/>
-      <c r="AC41" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD41" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC41" s="23"/>
+      <c r="AD41" s="46"/>
       <c r="AF41" s="54">
         <f ca="1">IF(M15="with and without cache", N14, FALSE)</f>
         <v>0</v>
@@ -5330,34 +5261,7 @@
       <c r="AG41" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="AH41">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI41" t="str">
-        <f ca="1"/>
-        <v>AF41</v>
-      </c>
-      <c r="AJ41" t="str">
-        <f ca="1"/>
-        <v>N14</v>
-      </c>
-      <c r="AK41" t="str">
-        <f ca="1"/>
-        <v>03_Third Link</v>
-      </c>
-      <c r="AM41" t="str">
-        <f ca="1"/>
-        <v>Third Link</v>
-      </c>
-      <c r="AO41" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP41" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP41" s="53"/>
     </row>
     <row r="42" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I42" s="22" t="s">
@@ -5388,36 +5292,15 @@
       <c r="U42" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="V42" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W42" s="23" t="str">
-        <f ca="1"/>
-        <v>T42</v>
-      </c>
-      <c r="X42" s="23" t="str">
-        <f ca="1"/>
-        <v>K18</v>
-      </c>
-      <c r="Y42" s="23" t="str">
-        <f ca="1"/>
-        <v>04_Fourth Link</v>
-      </c>
+      <c r="V42" s="23"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+      <c r="Y42" s="23"/>
       <c r="Z42" s="23"/>
-      <c r="AA42" s="23" t="str">
-        <f ca="1"/>
-        <v>Fourth Link</v>
-      </c>
+      <c r="AA42" s="23"/>
       <c r="AB42" s="23"/>
-      <c r="AC42" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD42" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC42" s="23"/>
+      <c r="AD42" s="46"/>
       <c r="AF42" s="54">
         <f ca="1">IF(M19="with and without cache", N18, FALSE)</f>
         <v>0</v>
@@ -5425,34 +5308,7 @@
       <c r="AG42" t="s">
         <v>64</v>
       </c>
-      <c r="AH42">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI42" t="str">
-        <f ca="1"/>
-        <v>AF42</v>
-      </c>
-      <c r="AJ42" t="str">
-        <f ca="1"/>
-        <v>N18</v>
-      </c>
-      <c r="AK42" t="str">
-        <f ca="1"/>
-        <v>04_Fourth Link</v>
-      </c>
-      <c r="AM42" t="str">
-        <f ca="1"/>
-        <v>Fourth Link</v>
-      </c>
-      <c r="AO42" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP42" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP42" s="53"/>
     </row>
     <row r="43" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I43" s="22" t="s">
@@ -5483,36 +5339,15 @@
       <c r="U43" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="V43" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W43" s="23" t="str">
-        <f ca="1"/>
-        <v>T43</v>
-      </c>
-      <c r="X43" s="23" t="str">
-        <f ca="1"/>
-        <v>K22</v>
-      </c>
-      <c r="Y43" s="23" t="str">
-        <f ca="1"/>
-        <v>05_Fifth Link</v>
-      </c>
+      <c r="V43" s="23"/>
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
       <c r="Z43" s="23"/>
-      <c r="AA43" s="23" t="str">
-        <f ca="1"/>
-        <v>Fifth Link</v>
-      </c>
+      <c r="AA43" s="23"/>
       <c r="AB43" s="23"/>
-      <c r="AC43" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD43" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC43" s="23"/>
+      <c r="AD43" s="46"/>
       <c r="AF43" s="54">
         <f ca="1">IF(M23="with and without cache", N22, FALSE)</f>
         <v>0</v>
@@ -5520,34 +5355,7 @@
       <c r="AG43" t="s">
         <v>65</v>
       </c>
-      <c r="AH43">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI43" t="str">
-        <f ca="1"/>
-        <v>AF43</v>
-      </c>
-      <c r="AJ43" t="str">
-        <f ca="1"/>
-        <v>N22</v>
-      </c>
-      <c r="AK43" t="str">
-        <f ca="1"/>
-        <v>05_Fifth Link</v>
-      </c>
-      <c r="AM43" t="str">
-        <f ca="1"/>
-        <v>Fifth Link</v>
-      </c>
-      <c r="AO43" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP43" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP43" s="53"/>
     </row>
     <row r="44" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I44" s="22" t="s">
@@ -5586,36 +5394,15 @@
       <c r="U44" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="V44" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W44" s="23" t="str">
-        <f ca="1"/>
-        <v>T44</v>
-      </c>
-      <c r="X44" s="23" t="str">
-        <f ca="1"/>
-        <v>K26</v>
-      </c>
-      <c r="Y44" s="23" t="str">
-        <f ca="1"/>
-        <v>06_Sixth Link</v>
-      </c>
+      <c r="V44" s="23"/>
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
       <c r="Z44" s="23"/>
-      <c r="AA44" s="23" t="str">
-        <f ca="1"/>
-        <v>Sixth Link</v>
-      </c>
+      <c r="AA44" s="23"/>
       <c r="AB44" s="23"/>
-      <c r="AC44" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD44" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC44" s="23"/>
+      <c r="AD44" s="46"/>
       <c r="AF44" s="54" t="b">
         <f ca="1">IF(M26="with and without cache", N26, FALSE)</f>
         <v>0</v>
@@ -5623,34 +5410,7 @@
       <c r="AG44" t="s">
         <v>66</v>
       </c>
-      <c r="AH44">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI44" t="str">
-        <f ca="1"/>
-        <v>AF45</v>
-      </c>
-      <c r="AJ44" t="str">
-        <f ca="1"/>
-        <v>N30</v>
-      </c>
-      <c r="AK44" t="str">
-        <f ca="1"/>
-        <v>07_Seventh Link</v>
-      </c>
-      <c r="AM44" t="str">
-        <f ca="1"/>
-        <v>Seventh Link</v>
-      </c>
-      <c r="AO44" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP44" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP44" s="53"/>
     </row>
     <row r="45" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I45" s="22" t="s">
@@ -5683,36 +5443,15 @@
       <c r="U45" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="V45" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W45" s="23" t="str">
-        <f ca="1"/>
-        <v>T45</v>
-      </c>
-      <c r="X45" s="23" t="str">
-        <f ca="1"/>
-        <v>K30</v>
-      </c>
-      <c r="Y45" s="23" t="str">
-        <f ca="1"/>
-        <v>07_Seventh Link</v>
-      </c>
+      <c r="V45" s="23"/>
+      <c r="W45" s="23"/>
+      <c r="X45" s="23"/>
+      <c r="Y45" s="23"/>
       <c r="Z45" s="23"/>
-      <c r="AA45" s="23" t="str">
-        <f ca="1"/>
-        <v>Seventh Link</v>
-      </c>
+      <c r="AA45" s="23"/>
       <c r="AB45" s="23"/>
-      <c r="AC45" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD45" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC45" s="23"/>
+      <c r="AD45" s="46"/>
       <c r="AF45" s="54">
         <f ca="1">IF(M31="with and without cache", N30, FALSE)</f>
         <v>0</v>
@@ -5720,34 +5459,7 @@
       <c r="AG45" t="s">
         <v>67</v>
       </c>
-      <c r="AH45">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI45" t="str">
-        <f ca="1"/>
-        <v>AF46</v>
-      </c>
-      <c r="AJ45" t="str">
-        <f ca="1"/>
-        <v>N34</v>
-      </c>
-      <c r="AK45" t="str">
-        <f ca="1"/>
-        <v>08_Eighth Link</v>
-      </c>
-      <c r="AM45" t="str">
-        <f ca="1"/>
-        <v>Eighth Link</v>
-      </c>
-      <c r="AO45" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP45" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP45" s="53"/>
     </row>
     <row r="46" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I46" s="22" t="s">
@@ -5768,36 +5480,15 @@
       <c r="U46" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="V46" s="48">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W46" s="48" t="str">
-        <f ca="1"/>
-        <v>T46</v>
-      </c>
-      <c r="X46" s="48" t="str">
-        <f ca="1"/>
-        <v>K34</v>
-      </c>
-      <c r="Y46" s="48" t="str">
-        <f ca="1"/>
-        <v>08_Eighth Link</v>
-      </c>
+      <c r="V46" s="48"/>
+      <c r="W46" s="48"/>
+      <c r="X46" s="48"/>
+      <c r="Y46" s="48"/>
       <c r="Z46" s="48"/>
-      <c r="AA46" s="48" t="str">
-        <f ca="1"/>
-        <v>Eighth Link</v>
-      </c>
+      <c r="AA46" s="48"/>
       <c r="AB46" s="48"/>
-      <c r="AC46" s="48" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD46" s="49" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC46" s="48"/>
+      <c r="AD46" s="49"/>
       <c r="AF46" s="56">
         <f ca="1">IF(M35="with and without cache", N34, FALSE)</f>
         <v>0</v>
@@ -5826,7 +5517,7 @@
       </c>
       <c r="AH47">
         <f ca="1">COUNT(AH39:AH46)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="9:42" x14ac:dyDescent="0.3">
@@ -5935,39 +5626,39 @@
       <c r="U50" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="V50" s="25" cm="1">
+      <c r="V50" s="25">
         <f t="array" aca="1" ref="V50" ca="1">_xlfn._xlws.FILTER(T50:T57, T50:T57=MAX(T50:T57))</f>
         <v>-1</v>
       </c>
-      <c r="W50" s="23" t="str" cm="1">
+      <c r="W50" s="23" t="str">
         <f t="array" aca="1" ref="W50" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(T50:T57), COLUMN(T50:T57), 4), T50:T57=MAX(T50:T57))</f>
         <v>T50</v>
       </c>
-      <c r="X50" s="23" t="str" cm="1">
+      <c r="X50" s="23" t="str">
         <f t="array" aca="1" ref="X50" ca="1">_xlfn._xlws.FILTER(U50:U57, T50:T57=MAX(T50:T57))</f>
         <v>K6</v>
       </c>
-      <c r="Y50" s="23" t="str" cm="1">
+      <c r="Y50" s="23" t="str">
         <f t="array" aca="1" ref="Y50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2))))</f>
         <v>01_First Link</v>
       </c>
       <c r="Z50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y50))</f>
+        <f t="array" aca="1" ref="Z50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y50))</f>
         <v>01_First Link</v>
       </c>
-      <c r="AA50" s="23" t="str" cm="1">
+      <c r="AA50" s="23" t="str">
         <f t="array" aca="1" ref="AA50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)))+1, 999)))</f>
         <v>First Link</v>
       </c>
       <c r="AB50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA50))</f>
+        <f t="array" aca="1" ref="AB50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA50))</f>
         <v>First Link</v>
       </c>
-      <c r="AC50" s="23" t="str" cm="1">
+      <c r="AC50" s="23" t="str">
         <f t="array" aca="1" ref="AC50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AD50" s="46" t="str" cm="1">
+      <c r="AD50" s="46" t="str">
         <f t="array" aca="1" ref="AD50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
@@ -5978,39 +5669,39 @@
       <c r="AG50" t="s">
         <v>61</v>
       </c>
-      <c r="AH50" s="25" cm="1">
+      <c r="AH50" s="25">
         <f t="array" aca="1" ref="AH50" ca="1">_xlfn._xlws.FILTER(AF50:AF57, AF50:AF57=MIN(AF50:AF57))</f>
         <v>99999</v>
       </c>
-      <c r="AI50" s="23" t="str" cm="1">
+      <c r="AI50" s="23" t="str">
         <f t="array" aca="1" ref="AI50" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(AF50:AF57), COLUMN(AF50:AF57), 4), AF50:AF57=MIN(AF50:AF57))</f>
         <v>AF50</v>
       </c>
-      <c r="AJ50" s="23" t="str" cm="1">
+      <c r="AJ50" s="23" t="str">
         <f t="array" aca="1" ref="AJ50" ca="1">_xlfn._xlws.FILTER(AG50:AG57, AF50:AF57=MIN(AF50:AF57))</f>
         <v>N6</v>
       </c>
-      <c r="AK50" s="23" t="str" cm="1">
+      <c r="AK50" s="23" t="str">
         <f t="array" aca="1" ref="AK50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5))))</f>
         <v>01_First Link</v>
       </c>
       <c r="AL50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AK50))</f>
+        <f t="array" aca="1" ref="AL50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AK50))</f>
         <v>01_First Link</v>
       </c>
-      <c r="AM50" s="23" t="str" cm="1">
+      <c r="AM50" s="23" t="str">
         <f t="array" aca="1" ref="AM50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)))+1, 999)))</f>
         <v>First Link</v>
       </c>
       <c r="AN50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AM50))</f>
+        <f t="array" aca="1" ref="AN50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AM50))</f>
         <v>First Link</v>
       </c>
-      <c r="AO50" s="23" t="str" cm="1">
+      <c r="AO50" s="23" t="str">
         <f t="array" aca="1" ref="AO50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AP50" s="46" t="str" cm="1">
+      <c r="AP50" s="46" t="str">
         <f t="array" aca="1" ref="AP50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
@@ -6259,7 +5950,7 @@
 IF(Formula_Sheet!V39&gt;=Formula_Sheet!V50,
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AA39),_xlfn.ANCHORARRAY( AC39),_xlfn.ANCHORARRAY( AD39), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))),
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AA50),_xlfn.ANCHORARRAY( AC50),_xlfn.ANCHORARRAY( AD50), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))))</f>
-        <v>The best recorded performance score was in the First Link page for Desktop devices with and without cache, Second Link page for Desktop devices with and without cache, Third Link page for Desktop devices with and without cache, Fourth Link page for Desktop devices with and without cache, Fifth Link page for Desktop devices with and without cache, Sixth Link page for Desktop devices with and without cache, Seventh Link page for Desktop devices with and without cache, Eighth Link page for Desktop devices with and without cache</v>
+        <v>The best recorded performance score was in the First Link page for Desktop devices with and without cache</v>
       </c>
       <c r="U61" s="59"/>
       <c r="V61" s="59"/>
@@ -6271,7 +5962,7 @@
 IF(Formula_Sheet!AH39&lt;=Formula_Sheet!AH50,
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AM39),_xlfn.ANCHORARRAY( AO39),_xlfn.ANCHORARRAY( AP39), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))),
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AM50),_xlfn.ANCHORARRAY( AO50),_xlfn.ANCHORARRAY( AP50), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))))</f>
-        <v>The worst recorded performance score was in the First Link page for Desktop devices with and without cache, Second Link page for Desktop devices with and without cache, Third Link page for Desktop devices with and without cache, Fourth Link page for Desktop devices with and without cache, Fifth Link page for Desktop devices with and without cache, Seventh Link page for Desktop devices with and without cache, Eighth Link page for Desktop devices with and without cache</v>
+        <v>The worst recorded performance score was in the First Link page for Desktop devices with and without cache</v>
       </c>
       <c r="AG61" s="60"/>
       <c r="AH61" s="60"/>
@@ -6292,11 +5983,11 @@
     <row r="64" spans="13:42" x14ac:dyDescent="0.3">
       <c r="T64" t="str">
         <f ca="1">"Refer to " &amp;IF(Formula_Sheet!V39&gt;=Formula_Sheet!V50, Formula_Sheet!Z39, Formula_Sheet!Z50)&amp; " tab for the best insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>Refer to 01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 06_Sixth Link, 07_Seventh Link, 08_Eighth Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
+        <v>Refer to 01_First Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
       <c r="AF64" t="str">
         <f ca="1">"Refer to " &amp;IF(Formula_Sheet!AH39&lt;=Formula_Sheet!AH50, Formula_Sheet!AL39, Formula_Sheet!AL50)&amp; " tab for the best insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>Refer to 01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 07_Seventh Link, 08_Eighth Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
+        <v>Refer to 01_First Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
     </row>
   </sheetData>
@@ -6331,18 +6022,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B7</f>
         <v>01_First Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6351,16 +6042,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6369,8 +6060,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6390,26 +6081,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="16"/>
@@ -6440,41 +6131,41 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6499,18 +6190,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B11</f>
         <v>02_Second Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6519,16 +6210,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6537,8 +6228,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6558,27 +6249,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -6622,28 +6313,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C30" s="21"/>
@@ -6684,18 +6375,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B15</f>
         <v>03_Third Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6704,16 +6395,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6722,8 +6413,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6743,27 +6434,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -6795,28 +6486,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -6858,18 +6549,18 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B19</f>
         <v>04_Fourth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6878,16 +6569,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6896,8 +6587,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6917,27 +6608,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -6981,28 +6672,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7043,18 +6734,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B23</f>
         <v>05_Fifth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7063,16 +6754,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7081,8 +6772,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7102,27 +6793,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -7166,28 +6857,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C29" s="21"/>
@@ -7228,18 +6919,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B27</f>
         <v>06_Sixth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7248,16 +6939,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7266,8 +6957,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7287,26 +6978,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
+      <c r="D9" s="86"/>
       <c r="E9" s="94"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="16"/>
@@ -7349,28 +7040,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7407,18 +7098,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B31</f>
         <v>07_Seventh Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7427,16 +7118,16 @@
       <c r="E3" s="33"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="35"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7445,8 +7136,8 @@
       <c r="E5" s="36"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7466,27 +7157,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -7518,28 +7209,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7576,18 +7267,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B35</f>
         <v>08_Eighth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7596,16 +7287,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7614,8 +7305,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7635,27 +7326,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -7699,28 +7390,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7740,6 +7431,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D539BB261075264EADE6FB64A6A44314" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8545620b90e3ca3b4fa9c0eed4ef96d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851fd863-1f96-44b1-878a-247793b557e9" xmlns:ns3="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2cedb268f8f7bfc874339ceeb7c9957" ns2:_="" ns3:_="">
     <xsd:import namespace="851fd863-1f96-44b1-878a-247793b557e9"/>
@@ -7968,17 +7670,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7989,6 +7680,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8007,23 +7715,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
refactor(excel): move module location and update complex formula to array in Formula_Sheet (#33)
- updated complex formula as array in Formula_Sheet to prevent errors when copying
- refactored module location for better structure
</commit_message>
<xml_diff>
--- a/template/excel-template.xlsx
+++ b/template/excel-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VonWebsterDLabajo\VS Code\Lighthouse-Playwright-Typescript-Automation\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F989AF-5DF9-4059-81CB-3096A2CA774B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA507479-F7D3-4D19-BB2E-1E68D51105C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3D68101-3EA1-4AB8-9C35-12A619CAE77F}"/>
   </bookViews>
@@ -1149,6 +1149,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1158,29 +1182,38 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1194,44 +1227,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1829,22 +1829,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="72"/>
+      <c r="E2" s="67"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="76"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="71"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1877,7 +1877,7 @@
       <c r="D6" s="61"/>
       <c r="E6" s="61"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="66" t="str">
+      <c r="G6" s="74" t="str">
         <f>IF(OR(ISBLANK(D6),ISBLANK(E6),TEXT(D6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D6,TEXT(E6,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E6),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K6=0,Formula_Sheet!N6=0),
@@ -1890,7 +1890,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="72" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1899,17 +1899,17 @@
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="67"/>
+      <c r="G7" s="75"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="70"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="68"/>
+      <c r="G8" s="76"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
@@ -1925,7 +1925,7 @@
       <c r="D10" s="61"/>
       <c r="E10" s="61"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="66" t="str">
+      <c r="G10" s="74" t="str">
         <f>IF(OR(ISBLANK(D10),ISBLANK(E10),TEXT(D10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D10,TEXT(E10,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E10),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K10=0,Formula_Sheet!N10=0),
@@ -1938,7 +1938,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="72" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1946,17 +1946,17 @@
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
-      <c r="G11" s="67"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="70"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="68"/>
+      <c r="G12" s="76"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
@@ -1972,7 +1972,7 @@
       <c r="D14" s="61"/>
       <c r="E14" s="61"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="66" t="str">
+      <c r="G14" s="74" t="str">
         <f>IF(OR(ISBLANK(D14),ISBLANK(E14),TEXT(D14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D14,TEXT(E14,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E14),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K14=0,Formula_Sheet!N14=0),
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="72" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1994,17 +1994,17 @@
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="67"/>
+      <c r="G15" s="75"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="70"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="68"/>
+      <c r="G16" s="76"/>
     </row>
     <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
@@ -2020,7 +2020,7 @@
       <c r="D18" s="63"/>
       <c r="E18" s="61"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="66" t="str">
+      <c r="G18" s="74" t="str">
         <f>IF(OR(ISBLANK(D18),ISBLANK(E18),TEXT(D18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D18,TEXT(E18,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E18),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K18=0,Formula_Sheet!N18=0),
@@ -2033,7 +2033,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="72" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -2042,17 +2042,17 @@
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="67"/>
+      <c r="G19" s="75"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="70"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="68"/>
+      <c r="G20" s="76"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
@@ -2068,7 +2068,7 @@
       <c r="D22" s="61"/>
       <c r="E22" s="61"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="66" t="str">
+      <c r="G22" s="74" t="str">
         <f>IF(OR(ISBLANK(D22),ISBLANK(E22),TEXT(D22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D22,TEXT(E22,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E22),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K22=0,Formula_Sheet!N22=0),
@@ -2081,7 +2081,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="72" t="s">
         <v>87</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -2090,17 +2090,17 @@
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="67"/>
+      <c r="G23" s="75"/>
     </row>
     <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="70"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="68"/>
+      <c r="G24" s="76"/>
     </row>
     <row r="25" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
@@ -2116,7 +2116,7 @@
       <c r="D26" s="61"/>
       <c r="E26" s="61"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="66" t="str">
+      <c r="G26" s="74" t="str">
         <f>IF(OR(ISBLANK(D26),ISBLANK(E26),TEXT(D26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D26,TEXT(E26,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E26),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K26=0,Formula_Sheet!N26=0),
@@ -2129,7 +2129,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="72" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -2138,17 +2138,17 @@
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="67"/>
+      <c r="G27" s="75"/>
     </row>
     <row r="28" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="70"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="68"/>
+      <c r="G28" s="76"/>
     </row>
     <row r="29" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
@@ -2164,7 +2164,7 @@
       <c r="D30" s="61"/>
       <c r="E30" s="63"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="66" t="str">
+      <c r="G30" s="74" t="str">
         <f>IF(OR(ISBLANK(D30),ISBLANK(E30),TEXT(D30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D30,TEXT(E30,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E30),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K30=0,Formula_Sheet!N30=0),
@@ -2177,7 +2177,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="72" t="s">
         <v>89</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -2186,17 +2186,17 @@
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="67"/>
+      <c r="G31" s="75"/>
     </row>
     <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="70"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="68"/>
+      <c r="G32" s="76"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
@@ -2212,7 +2212,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="63"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="66" t="str">
+      <c r="G34" s="74" t="str">
         <f>IF(OR(ISBLANK(D34),ISBLANK(E34),TEXT(D34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;D34,TEXT(E34,"mmmm d, yyyy, h:mm:ss am/pm")&lt;&gt;E34),
 "Kindly add Analysis Timestamp!",
 IF(OR(Formula_Sheet!K34=0,Formula_Sheet!N34=0),
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="69" t="s">
+      <c r="B35" s="72" t="s">
         <v>90</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -2234,17 +2234,17 @@
       <c r="D35" s="43"/>
       <c r="E35" s="43"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="67"/>
+      <c r="G35" s="75"/>
     </row>
     <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="70"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="68"/>
+      <c r="G36" s="76"/>
     </row>
     <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
@@ -2260,7 +2260,7 @@
         <v>16</v>
       </c>
       <c r="F38" s="6"/>
-      <c r="G38" s="66" t="str">
+      <c r="G38" s="74" t="str">
         <f>IF(OR(Formula_Sheet!J39=0,Formula_Sheet!K39=0),
 "Kindly, fill the Performance Score first!",
 Formula_Sheet!T61 &amp; Formula_Sheet!T62 &amp;
@@ -2282,7 +2282,7 @@
         <v>19</v>
       </c>
       <c r="F39" s="6"/>
-      <c r="G39" s="67"/>
+      <c r="G39" s="75"/>
     </row>
     <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="13" t="s">
@@ -2292,21 +2292,16 @@
         <v>22</v>
       </c>
       <c r="F40" s="6"/>
-      <c r="G40" s="67"/>
+      <c r="G40" s="75"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G41" s="67"/>
+      <c r="G41" s="75"/>
     </row>
     <row r="42" spans="2:7" ht="64.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G42" s="68"/>
+      <c r="G42" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="G38:G42"/>
@@ -2322,6 +2317,11 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="G14:G16"/>
     <mergeCell ref="G10:G12"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E8">
     <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
@@ -2421,8 +2421,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="I3:AP64"/>
   <sheetViews>
-    <sheetView topLeftCell="W43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF50" sqref="AF50"/>
+    <sheetView topLeftCell="S27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V50" sqref="V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5101,40 +5101,40 @@
       <c r="U39" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="V39" s="23" cm="1">
-        <f t="array" aca="1" ref="V39:V46" ca="1">_xlfn._xlws.FILTER(T39:T46, T39:T46=MAX(T39:T46))</f>
-        <v>0</v>
-      </c>
-      <c r="W39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="W39:W46" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(T39:T46), COLUMN(T39:T46), 4), T39:T46=MAX(T39:T46))</f>
+      <c r="V39" s="23">
+        <f t="array" aca="1" ref="V39" ca="1">_xlfn._xlws.FILTER(T39:T46, T39:T46=MAX(T39:T46))</f>
+        <v>0</v>
+      </c>
+      <c r="W39" s="23" t="str">
+        <f t="array" aca="1" ref="W39" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(T39:T46), COLUMN(T39:T46), 4), T39:T46=MAX(T39:T46))</f>
         <v>T39</v>
       </c>
-      <c r="X39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="X39:X46" ca="1">_xlfn._xlws.FILTER(U39:U46, T39:T46=MAX(T39:T46))</f>
+      <c r="X39" s="23" t="str">
+        <f t="array" aca="1" ref="X39" ca="1">_xlfn._xlws.FILTER(U39:U46, T39:T46=MAX(T39:T46))</f>
         <v>K6</v>
       </c>
-      <c r="Y39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="Y39:Y46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2))))</f>
+      <c r="Y39" s="23" t="str">
+        <f t="array" aca="1" ref="Y39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2))))</f>
         <v>01_First Link</v>
       </c>
       <c r="Z39" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y39))</f>
-        <v>01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 06_Sixth Link, 07_Seventh Link, 08_Eighth Link</v>
-      </c>
-      <c r="AA39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="AA39:AA46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)))+1, 999)))</f>
+        <f t="array" aca="1" ref="Z39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y39))</f>
+        <v>01_First Link</v>
+      </c>
+      <c r="AA39" s="23" t="str">
+        <f t="array" aca="1" ref="AA39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)))+1, 999)))</f>
         <v>First Link</v>
       </c>
       <c r="AB39" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA39))</f>
-        <v>First Link, Second Link, Third Link, Fourth Link, Fifth Link, Sixth Link, Seventh Link, Eighth Link</v>
-      </c>
-      <c r="AC39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="AC39:AC46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+        <f t="array" aca="1" ref="AB39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA39))</f>
+        <v>First Link</v>
+      </c>
+      <c r="AC39" s="23" t="str">
+        <f t="array" aca="1" ref="AC39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AD39" s="46" t="str" cm="1">
-        <f t="array" aca="1" ref="AD39:AD46" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+      <c r="AD39" s="46" t="str">
+        <f t="array" aca="1" ref="AD39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
       <c r="AF39" s="54">
@@ -5144,40 +5144,40 @@
       <c r="AG39" t="s">
         <v>61</v>
       </c>
-      <c r="AH39" cm="1">
-        <f t="array" aca="1" ref="AH39:AH45" ca="1">_xlfn._xlws.FILTER(AF39:AF46, AF39:AF46=MIN(AF39:AF46))</f>
-        <v>0</v>
-      </c>
-      <c r="AI39" t="str" cm="1">
-        <f t="array" aca="1" ref="AI39:AI45" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(AF39:AF46), COLUMN(AF39:AF46), 4), AF39:AF46=MIN(AF39:AF46))</f>
+      <c r="AH39">
+        <f t="array" aca="1" ref="AH39" ca="1">_xlfn._xlws.FILTER(AF39:AF46, AF39:AF46=MIN(AF39:AF46))</f>
+        <v>0</v>
+      </c>
+      <c r="AI39" t="str">
+        <f t="array" aca="1" ref="AI39" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(AF39:AF46), COLUMN(AF39:AF46), 4), AF39:AF46=MIN(AF39:AF46))</f>
         <v>AF39</v>
       </c>
-      <c r="AJ39" t="str" cm="1">
-        <f t="array" aca="1" ref="AJ39:AJ45" ca="1">_xlfn._xlws.FILTER(AG39:AG46, AF39:AF46=MIN(AF39:AF46))</f>
+      <c r="AJ39" t="str">
+        <f t="array" aca="1" ref="AJ39" ca="1">_xlfn._xlws.FILTER(AG39:AG46, AF39:AF46=MIN(AF39:AF46))</f>
         <v>N6</v>
       </c>
-      <c r="AK39" t="str" cm="1">
-        <f t="array" aca="1" ref="AK39:AK45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5))))</f>
+      <c r="AK39" t="str">
+        <f t="array" aca="1" ref="AK39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5))))</f>
         <v>01_First Link</v>
       </c>
       <c r="AL39" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE, AK39, AK40, AK41, AK42, AK43, AK44, AK45, AK46)</f>
-        <v>01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 07_Seventh Link, 08_Eighth Link</v>
-      </c>
-      <c r="AM39" t="str" cm="1">
-        <f t="array" aca="1" ref="AM39:AM45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)))+1, 999)))</f>
+        <f t="array" aca="1" ref="AL39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AK39))</f>
+        <v>01_First Link</v>
+      </c>
+      <c r="AM39" t="str">
+        <f t="array" aca="1" ref="AM39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39),_xlfn.LAMBDA(_xlpm.cell_address,MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1,COLUMN(INDIRECT(_xlpm.cell_address))-5)),FIND("_",INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1,COLUMN(INDIRECT(_xlpm.cell_address))-5)))+1,999)))</f>
         <v>First Link</v>
       </c>
       <c r="AN39" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE, AM39, AM40, AM41, AM42, AM43, AM44, AM45, AM46)</f>
-        <v>First Link, Second Link, Third Link, Fourth Link, Fifth Link, Seventh Link, Eighth Link</v>
-      </c>
-      <c r="AO39" s="23" t="str" cm="1">
-        <f t="array" aca="1" ref="AO39:AO45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+        <f t="array" aca="1" ref="AN39" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AM39))</f>
+        <v>First Link</v>
+      </c>
+      <c r="AO39" s="23" t="str">
+        <f t="array" aca="1" ref="AO39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AP39" s="46" t="str" cm="1">
-        <f t="array" aca="1" ref="AP39:AP45" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
+      <c r="AP39" s="46" t="str">
+        <f t="array" aca="1" ref="AP39" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ39), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
     </row>
@@ -5204,36 +5204,15 @@
       <c r="U40" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="V40" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W40" s="23" t="str">
-        <f ca="1"/>
-        <v>T40</v>
-      </c>
-      <c r="X40" s="23" t="str">
-        <f ca="1"/>
-        <v>K10</v>
-      </c>
-      <c r="Y40" s="23" t="str">
-        <f ca="1"/>
-        <v>02_Second Link</v>
-      </c>
+      <c r="V40" s="23"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
       <c r="Z40" s="23"/>
-      <c r="AA40" s="23" t="str">
-        <f ca="1"/>
-        <v>Second Link</v>
-      </c>
+      <c r="AA40" s="23"/>
       <c r="AB40" s="23"/>
-      <c r="AC40" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD40" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC40" s="23"/>
+      <c r="AD40" s="46"/>
       <c r="AF40" s="54">
         <f ca="1">IF(M11="with and without cache", N10, FALSE)</f>
         <v>0</v>
@@ -5241,34 +5220,7 @@
       <c r="AG40" t="s">
         <v>62</v>
       </c>
-      <c r="AH40">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI40" t="str">
-        <f ca="1"/>
-        <v>AF40</v>
-      </c>
-      <c r="AJ40" t="str">
-        <f ca="1"/>
-        <v>N10</v>
-      </c>
-      <c r="AK40" t="str">
-        <f ca="1"/>
-        <v>02_Second Link</v>
-      </c>
-      <c r="AM40" t="str">
-        <f ca="1"/>
-        <v>Second Link</v>
-      </c>
-      <c r="AO40" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP40" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP40" s="53"/>
     </row>
     <row r="41" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I41" s="22" t="s">
@@ -5293,36 +5245,15 @@
       <c r="U41" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="V41" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W41" s="23" t="str">
-        <f ca="1"/>
-        <v>T41</v>
-      </c>
-      <c r="X41" s="23" t="str">
-        <f ca="1"/>
-        <v>K14</v>
-      </c>
-      <c r="Y41" s="23" t="str">
-        <f ca="1"/>
-        <v>03_Third Link</v>
-      </c>
+      <c r="V41" s="23"/>
+      <c r="W41" s="23"/>
+      <c r="X41" s="23"/>
+      <c r="Y41" s="23"/>
       <c r="Z41" s="23"/>
-      <c r="AA41" s="23" t="str">
-        <f ca="1"/>
-        <v>Third Link</v>
-      </c>
+      <c r="AA41" s="23"/>
       <c r="AB41" s="23"/>
-      <c r="AC41" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD41" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC41" s="23"/>
+      <c r="AD41" s="46"/>
       <c r="AF41" s="54">
         <f ca="1">IF(M15="with and without cache", N14, FALSE)</f>
         <v>0</v>
@@ -5330,34 +5261,7 @@
       <c r="AG41" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="AH41">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI41" t="str">
-        <f ca="1"/>
-        <v>AF41</v>
-      </c>
-      <c r="AJ41" t="str">
-        <f ca="1"/>
-        <v>N14</v>
-      </c>
-      <c r="AK41" t="str">
-        <f ca="1"/>
-        <v>03_Third Link</v>
-      </c>
-      <c r="AM41" t="str">
-        <f ca="1"/>
-        <v>Third Link</v>
-      </c>
-      <c r="AO41" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP41" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP41" s="53"/>
     </row>
     <row r="42" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I42" s="22" t="s">
@@ -5388,36 +5292,15 @@
       <c r="U42" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="V42" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W42" s="23" t="str">
-        <f ca="1"/>
-        <v>T42</v>
-      </c>
-      <c r="X42" s="23" t="str">
-        <f ca="1"/>
-        <v>K18</v>
-      </c>
-      <c r="Y42" s="23" t="str">
-        <f ca="1"/>
-        <v>04_Fourth Link</v>
-      </c>
+      <c r="V42" s="23"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+      <c r="Y42" s="23"/>
       <c r="Z42" s="23"/>
-      <c r="AA42" s="23" t="str">
-        <f ca="1"/>
-        <v>Fourth Link</v>
-      </c>
+      <c r="AA42" s="23"/>
       <c r="AB42" s="23"/>
-      <c r="AC42" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD42" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC42" s="23"/>
+      <c r="AD42" s="46"/>
       <c r="AF42" s="54">
         <f ca="1">IF(M19="with and without cache", N18, FALSE)</f>
         <v>0</v>
@@ -5425,34 +5308,7 @@
       <c r="AG42" t="s">
         <v>64</v>
       </c>
-      <c r="AH42">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI42" t="str">
-        <f ca="1"/>
-        <v>AF42</v>
-      </c>
-      <c r="AJ42" t="str">
-        <f ca="1"/>
-        <v>N18</v>
-      </c>
-      <c r="AK42" t="str">
-        <f ca="1"/>
-        <v>04_Fourth Link</v>
-      </c>
-      <c r="AM42" t="str">
-        <f ca="1"/>
-        <v>Fourth Link</v>
-      </c>
-      <c r="AO42" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP42" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP42" s="53"/>
     </row>
     <row r="43" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I43" s="22" t="s">
@@ -5483,36 +5339,15 @@
       <c r="U43" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="V43" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W43" s="23" t="str">
-        <f ca="1"/>
-        <v>T43</v>
-      </c>
-      <c r="X43" s="23" t="str">
-        <f ca="1"/>
-        <v>K22</v>
-      </c>
-      <c r="Y43" s="23" t="str">
-        <f ca="1"/>
-        <v>05_Fifth Link</v>
-      </c>
+      <c r="V43" s="23"/>
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
       <c r="Z43" s="23"/>
-      <c r="AA43" s="23" t="str">
-        <f ca="1"/>
-        <v>Fifth Link</v>
-      </c>
+      <c r="AA43" s="23"/>
       <c r="AB43" s="23"/>
-      <c r="AC43" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD43" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC43" s="23"/>
+      <c r="AD43" s="46"/>
       <c r="AF43" s="54">
         <f ca="1">IF(M23="with and without cache", N22, FALSE)</f>
         <v>0</v>
@@ -5520,34 +5355,7 @@
       <c r="AG43" t="s">
         <v>65</v>
       </c>
-      <c r="AH43">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI43" t="str">
-        <f ca="1"/>
-        <v>AF43</v>
-      </c>
-      <c r="AJ43" t="str">
-        <f ca="1"/>
-        <v>N22</v>
-      </c>
-      <c r="AK43" t="str">
-        <f ca="1"/>
-        <v>05_Fifth Link</v>
-      </c>
-      <c r="AM43" t="str">
-        <f ca="1"/>
-        <v>Fifth Link</v>
-      </c>
-      <c r="AO43" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP43" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP43" s="53"/>
     </row>
     <row r="44" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I44" s="22" t="s">
@@ -5586,36 +5394,15 @@
       <c r="U44" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="V44" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W44" s="23" t="str">
-        <f ca="1"/>
-        <v>T44</v>
-      </c>
-      <c r="X44" s="23" t="str">
-        <f ca="1"/>
-        <v>K26</v>
-      </c>
-      <c r="Y44" s="23" t="str">
-        <f ca="1"/>
-        <v>06_Sixth Link</v>
-      </c>
+      <c r="V44" s="23"/>
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
       <c r="Z44" s="23"/>
-      <c r="AA44" s="23" t="str">
-        <f ca="1"/>
-        <v>Sixth Link</v>
-      </c>
+      <c r="AA44" s="23"/>
       <c r="AB44" s="23"/>
-      <c r="AC44" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD44" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC44" s="23"/>
+      <c r="AD44" s="46"/>
       <c r="AF44" s="54" t="b">
         <f ca="1">IF(M26="with and without cache", N26, FALSE)</f>
         <v>0</v>
@@ -5623,34 +5410,7 @@
       <c r="AG44" t="s">
         <v>66</v>
       </c>
-      <c r="AH44">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI44" t="str">
-        <f ca="1"/>
-        <v>AF45</v>
-      </c>
-      <c r="AJ44" t="str">
-        <f ca="1"/>
-        <v>N30</v>
-      </c>
-      <c r="AK44" t="str">
-        <f ca="1"/>
-        <v>07_Seventh Link</v>
-      </c>
-      <c r="AM44" t="str">
-        <f ca="1"/>
-        <v>Seventh Link</v>
-      </c>
-      <c r="AO44" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP44" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP44" s="53"/>
     </row>
     <row r="45" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I45" s="22" t="s">
@@ -5683,36 +5443,15 @@
       <c r="U45" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="V45" s="23">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W45" s="23" t="str">
-        <f ca="1"/>
-        <v>T45</v>
-      </c>
-      <c r="X45" s="23" t="str">
-        <f ca="1"/>
-        <v>K30</v>
-      </c>
-      <c r="Y45" s="23" t="str">
-        <f ca="1"/>
-        <v>07_Seventh Link</v>
-      </c>
+      <c r="V45" s="23"/>
+      <c r="W45" s="23"/>
+      <c r="X45" s="23"/>
+      <c r="Y45" s="23"/>
       <c r="Z45" s="23"/>
-      <c r="AA45" s="23" t="str">
-        <f ca="1"/>
-        <v>Seventh Link</v>
-      </c>
+      <c r="AA45" s="23"/>
       <c r="AB45" s="23"/>
-      <c r="AC45" s="23" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD45" s="46" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC45" s="23"/>
+      <c r="AD45" s="46"/>
       <c r="AF45" s="54">
         <f ca="1">IF(M31="with and without cache", N30, FALSE)</f>
         <v>0</v>
@@ -5720,34 +5459,7 @@
       <c r="AG45" t="s">
         <v>67</v>
       </c>
-      <c r="AH45">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI45" t="str">
-        <f ca="1"/>
-        <v>AF46</v>
-      </c>
-      <c r="AJ45" t="str">
-        <f ca="1"/>
-        <v>N34</v>
-      </c>
-      <c r="AK45" t="str">
-        <f ca="1"/>
-        <v>08_Eighth Link</v>
-      </c>
-      <c r="AM45" t="str">
-        <f ca="1"/>
-        <v>Eighth Link</v>
-      </c>
-      <c r="AO45" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AP45" s="53" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AP45" s="53"/>
     </row>
     <row r="46" spans="9:42" x14ac:dyDescent="0.3">
       <c r="I46" s="22" t="s">
@@ -5768,36 +5480,15 @@
       <c r="U46" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="V46" s="48">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="W46" s="48" t="str">
-        <f ca="1"/>
-        <v>T46</v>
-      </c>
-      <c r="X46" s="48" t="str">
-        <f ca="1"/>
-        <v>K34</v>
-      </c>
-      <c r="Y46" s="48" t="str">
-        <f ca="1"/>
-        <v>08_Eighth Link</v>
-      </c>
+      <c r="V46" s="48"/>
+      <c r="W46" s="48"/>
+      <c r="X46" s="48"/>
+      <c r="Y46" s="48"/>
       <c r="Z46" s="48"/>
-      <c r="AA46" s="48" t="str">
-        <f ca="1"/>
-        <v>Eighth Link</v>
-      </c>
+      <c r="AA46" s="48"/>
       <c r="AB46" s="48"/>
-      <c r="AC46" s="48" t="str">
-        <f ca="1"/>
-        <v>Desktop</v>
-      </c>
-      <c r="AD46" s="49" t="str">
-        <f ca="1"/>
-        <v>with and without cache</v>
-      </c>
+      <c r="AC46" s="48"/>
+      <c r="AD46" s="49"/>
       <c r="AF46" s="56">
         <f ca="1">IF(M35="with and without cache", N34, FALSE)</f>
         <v>0</v>
@@ -5826,7 +5517,7 @@
       </c>
       <c r="AH47">
         <f ca="1">COUNT(AH39:AH46)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="9:42" x14ac:dyDescent="0.3">
@@ -5935,39 +5626,39 @@
       <c r="U50" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="V50" s="25" cm="1">
+      <c r="V50" s="25">
         <f t="array" aca="1" ref="V50" ca="1">_xlfn._xlws.FILTER(T50:T57, T50:T57=MAX(T50:T57))</f>
         <v>-1</v>
       </c>
-      <c r="W50" s="23" t="str" cm="1">
+      <c r="W50" s="23" t="str">
         <f t="array" aca="1" ref="W50" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(T50:T57), COLUMN(T50:T57), 4), T50:T57=MAX(T50:T57))</f>
         <v>T50</v>
       </c>
-      <c r="X50" s="23" t="str" cm="1">
+      <c r="X50" s="23" t="str">
         <f t="array" aca="1" ref="X50" ca="1">_xlfn._xlws.FILTER(U50:U57, T50:T57=MAX(T50:T57))</f>
         <v>K6</v>
       </c>
-      <c r="Y50" s="23" t="str" cm="1">
+      <c r="Y50" s="23" t="str">
         <f t="array" aca="1" ref="Y50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2))))</f>
         <v>01_First Link</v>
       </c>
       <c r="Z50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y50))</f>
+        <f t="array" aca="1" ref="Z50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( Y50))</f>
         <v>01_First Link</v>
       </c>
-      <c r="AA50" s="23" t="str" cm="1">
+      <c r="AA50" s="23" t="str">
         <f t="array" aca="1" ref="AA50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-2)))+1, 999)))</f>
         <v>First Link</v>
       </c>
       <c r="AB50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA50))</f>
+        <f t="array" aca="1" ref="AB50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AA50))</f>
         <v>First Link</v>
       </c>
-      <c r="AC50" s="23" t="str" cm="1">
+      <c r="AC50" s="23" t="str">
         <f t="array" aca="1" ref="AC50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AD50" s="46" t="str" cm="1">
+      <c r="AD50" s="46" t="str">
         <f t="array" aca="1" ref="AD50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(X50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
@@ -5978,39 +5669,39 @@
       <c r="AG50" t="s">
         <v>61</v>
       </c>
-      <c r="AH50" s="25" cm="1">
+      <c r="AH50" s="25">
         <f t="array" aca="1" ref="AH50" ca="1">_xlfn._xlws.FILTER(AF50:AF57, AF50:AF57=MIN(AF50:AF57))</f>
         <v>99999</v>
       </c>
-      <c r="AI50" s="23" t="str" cm="1">
+      <c r="AI50" s="23" t="str">
         <f t="array" aca="1" ref="AI50" ca="1">_xlfn._xlws.FILTER(ADDRESS(ROW(AF50:AF57), COLUMN(AF50:AF57), 4), AF50:AF57=MIN(AF50:AF57))</f>
         <v>AF50</v>
       </c>
-      <c r="AJ50" s="23" t="str" cm="1">
+      <c r="AJ50" s="23" t="str">
         <f t="array" aca="1" ref="AJ50" ca="1">_xlfn._xlws.FILTER(AG50:AG57, AF50:AF57=MIN(AF50:AF57))</f>
         <v>N6</v>
       </c>
-      <c r="AK50" s="23" t="str" cm="1">
+      <c r="AK50" s="23" t="str">
         <f t="array" aca="1" ref="AK50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5))))</f>
         <v>01_First Link</v>
       </c>
       <c r="AL50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AK50))</f>
+        <f t="array" aca="1" ref="AL50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AK50))</f>
         <v>01_First Link</v>
       </c>
-      <c r="AM50" s="23" t="str" cm="1">
+      <c r="AM50" s="23" t="str">
         <f t="array" aca="1" ref="AM50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, MID(INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)), FIND("_", INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))-1, COLUMN(INDIRECT(_xlpm.cell_address))-5)))+1, 999)))</f>
         <v>First Link</v>
       </c>
       <c r="AN50" s="23" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AM50))</f>
+        <f t="array" aca="1" ref="AN50" ca="1">_xlfn.TEXTJOIN(", ", TRUE,_xlfn.ANCHORARRAY( AM50))</f>
         <v>First Link</v>
       </c>
-      <c r="AO50" s="23" t="str" cm="1">
+      <c r="AO50" s="23" t="str">
         <f t="array" aca="1" ref="AO50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address)), COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>Desktop</v>
       </c>
-      <c r="AP50" s="46" t="str" cm="1">
+      <c r="AP50" s="46" t="str">
         <f t="array" aca="1" ref="AP50" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(AJ50), _xlfn.LAMBDA(_xlpm.cell_address, INDIRECT(ADDRESS(ROW(INDIRECT(_xlpm.cell_address))+1, COLUMN(INDIRECT(_xlpm.cell_address))-1))))</f>
         <v>with and without cache</v>
       </c>
@@ -6259,7 +5950,7 @@
 IF(Formula_Sheet!V39&gt;=Formula_Sheet!V50,
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AA39),_xlfn.ANCHORARRAY( AC39),_xlfn.ANCHORARRAY( AD39), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))),
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AA50),_xlfn.ANCHORARRAY( AC50),_xlfn.ANCHORARRAY( AD50), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))))</f>
-        <v>The best recorded performance score was in the First Link page for Desktop devices with and without cache, Second Link page for Desktop devices with and without cache, Third Link page for Desktop devices with and without cache, Fourth Link page for Desktop devices with and without cache, Fifth Link page for Desktop devices with and without cache, Sixth Link page for Desktop devices with and without cache, Seventh Link page for Desktop devices with and without cache, Eighth Link page for Desktop devices with and without cache</v>
+        <v>The best recorded performance score was in the First Link page for Desktop devices with and without cache</v>
       </c>
       <c r="U61" s="59"/>
       <c r="V61" s="59"/>
@@ -6271,7 +5962,7 @@
 IF(Formula_Sheet!AH39&lt;=Formula_Sheet!AH50,
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AM39),_xlfn.ANCHORARRAY( AO39),_xlfn.ANCHORARRAY( AP39), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))),
 _xlfn.TEXTJOIN(", ", TRUE, _xlfn.MAP(_xlfn.ANCHORARRAY(AM50),_xlfn.ANCHORARRAY( AO50),_xlfn.ANCHORARRAY( AP50), _xlfn.LAMBDA(_xlpm.name,_xlpm.device,_xlpm.cache, _xlpm.name &amp; " page for " &amp; _xlpm.device &amp; " devices " &amp; _xlpm.cache))))</f>
-        <v>The worst recorded performance score was in the First Link page for Desktop devices with and without cache, Second Link page for Desktop devices with and without cache, Third Link page for Desktop devices with and without cache, Fourth Link page for Desktop devices with and without cache, Fifth Link page for Desktop devices with and without cache, Seventh Link page for Desktop devices with and without cache, Eighth Link page for Desktop devices with and without cache</v>
+        <v>The worst recorded performance score was in the First Link page for Desktop devices with and without cache</v>
       </c>
       <c r="AG61" s="60"/>
       <c r="AH61" s="60"/>
@@ -6292,11 +5983,11 @@
     <row r="64" spans="13:42" x14ac:dyDescent="0.3">
       <c r="T64" t="str">
         <f ca="1">"Refer to " &amp;IF(Formula_Sheet!V39&gt;=Formula_Sheet!V50, Formula_Sheet!Z39, Formula_Sheet!Z50)&amp; " tab for the best insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>Refer to 01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 06_Sixth Link, 07_Seventh Link, 08_Eighth Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
+        <v>Refer to 01_First Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
       <c r="AF64" t="str">
         <f ca="1">"Refer to " &amp;IF(Formula_Sheet!AH39&lt;=Formula_Sheet!AH50, Formula_Sheet!AL39, Formula_Sheet!AL50)&amp; " tab for the best insight, links for full diagnostic readings and recommendations for improvement."</f>
-        <v>Refer to 01_First Link, 02_Second Link, 03_Third Link, 04_Fourth Link, 05_Fifth Link, 07_Seventh Link, 08_Eighth Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
+        <v>Refer to 01_First Link tab for the best insight, links for full diagnostic readings and recommendations for improvement.</v>
       </c>
     </row>
   </sheetData>
@@ -6331,18 +6022,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D6</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B7</f>
         <v>01_First Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6351,16 +6042,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6369,8 +6060,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6390,26 +6081,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="16"/>
@@ -6440,41 +6131,41 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6499,18 +6190,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D10</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B11</f>
         <v>02_Second Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6519,16 +6210,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6537,8 +6228,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6558,27 +6249,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -6622,28 +6313,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C30" s="21"/>
@@ -6684,18 +6375,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D14</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B15</f>
         <v>03_Third Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6704,16 +6395,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6722,8 +6413,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6743,27 +6434,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -6795,28 +6486,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -6858,18 +6549,18 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D18</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B19</f>
         <v>04_Fourth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -6878,16 +6569,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -6896,8 +6587,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -6917,27 +6608,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -6981,28 +6672,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7043,18 +6734,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D22</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B23</f>
         <v>05_Fifth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7063,16 +6754,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7081,8 +6772,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7102,27 +6793,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -7166,28 +6857,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C29" s="21"/>
@@ -7228,18 +6919,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D26</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B27</f>
         <v>06_Sixth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7248,16 +6939,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7266,8 +6957,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7287,26 +6978,26 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
+      <c r="D9" s="86"/>
       <c r="E9" s="94"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="16"/>
@@ -7349,28 +7040,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7407,18 +7098,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D30</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B31</f>
         <v>07_Seventh Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7427,16 +7118,16 @@
       <c r="E3" s="33"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="35"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7445,8 +7136,8 @@
       <c r="E5" s="36"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7466,27 +7157,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -7518,28 +7209,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7576,18 +7267,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="86">
+      <c r="C2" s="77">
         <f>Summary!D34</f>
         <v>0</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="79" t="str">
         <f>Summary!B35</f>
         <v>08_Eighth Link</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="82" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7596,16 +7287,16 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="89"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="83"/>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="89"/>
-      <c r="C5" s="92" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -7614,8 +7305,8 @@
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="93"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7635,27 +7326,27 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="87"/>
     </row>
     <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -7699,28 +7390,28 @@
       <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="85">
         <f>E5</f>
         <v>0</v>
       </c>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
     </row>
     <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="89"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7740,6 +7431,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D539BB261075264EADE6FB64A6A44314" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8545620b90e3ca3b4fa9c0eed4ef96d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851fd863-1f96-44b1-878a-247793b557e9" xmlns:ns3="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2cedb268f8f7bfc874339ceeb7c9957" ns2:_="" ns3:_="">
     <xsd:import namespace="851fd863-1f96-44b1-878a-247793b557e9"/>
@@ -7968,17 +7670,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851fd863-1f96-44b1-878a-247793b557e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7989,6 +7680,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
+    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F5D0948-37AE-4A53-8E3A-E23AA9EDC499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8007,23 +7715,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2192765-7A29-43CE-B5C9-BF081AEF5ED1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="2d55a6ab-b9f4-4be6-b06a-2cc46fdc62a1"/>
-    <ds:schemaRef ds:uri="851fd863-1f96-44b1-878a-247793b557e9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6E2078-3560-474E-801B-A28E523CFF9F}">
   <ds:schemaRefs>

</xml_diff>